<commit_message>
Added data on 3 Aug
</commit_message>
<xml_diff>
--- a/Araraquara_covid.xlsx
+++ b/Araraquara_covid.xlsx
@@ -6,11 +6,11 @@
     <sheet state="visible" name="Araraquara covid.csv" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="Z_8C5E459B_F781_4902_BF57_DF5AFCFB730D_.wvu.FilterData">'Araraquara covid.csv'!$G$9</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_35B53A02_2CED_4375_A753_341DF5F2FA7E_.wvu.FilterData">'Araraquara covid.csv'!$G$9</definedName>
   </definedNames>
   <calcPr/>
   <customWorkbookViews>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{8C5E459B-F781-4902-BF57-DF5AFCFB730D}" name="Filtro 1"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{35B53A02-2CED-4375-A753-341DF5F2FA7E}" name="Filtro 1"/>
   </customWorkbookViews>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
@@ -95,7 +95,7 @@
   </commentList>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7miLvMMOgJDvb3YLSuOImfaGAriPRw=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mgXH8Yftvi4L0xY/EXwvbq6Pt1r/A=="/>
     </ext>
   </extLst>
 </comments>
@@ -206,7 +206,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="16">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -253,12 +253,6 @@
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="5" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -574,7 +568,7 @@
         <v>5.0</v>
       </c>
       <c r="D3" s="2">
-        <f t="shared" ref="D3:D489" si="2">(C3-C2)</f>
+        <f t="shared" ref="D3:D492" si="2">(C3-C2)</f>
         <v>2</v>
       </c>
       <c r="E3" s="1">
@@ -15398,35 +15392,35 @@
       <c r="B488" s="4">
         <v>44407.0</v>
       </c>
-      <c r="C488" s="15">
+      <c r="C488" s="1">
         <v>28135.0</v>
       </c>
       <c r="D488" s="2">
         <f t="shared" si="2"/>
         <v>31</v>
       </c>
-      <c r="E488" s="15">
+      <c r="E488" s="1">
         <v>560.0</v>
       </c>
-      <c r="F488" s="15">
+      <c r="F488" s="1">
         <v>98.0</v>
       </c>
-      <c r="G488" s="15">
+      <c r="G488" s="1">
         <v>97.0</v>
       </c>
-      <c r="H488" s="15">
+      <c r="H488" s="1">
         <v>49.0</v>
       </c>
-      <c r="I488" s="16">
+      <c r="I488" s="14">
         <v>144080.0</v>
       </c>
-      <c r="J488" s="15">
+      <c r="J488" s="1">
         <v>54367.0</v>
       </c>
-      <c r="K488" s="15">
+      <c r="K488" s="1">
         <v>5884.0</v>
       </c>
-      <c r="L488" s="15">
+      <c r="L488" s="1">
         <v>204336.0</v>
       </c>
     </row>
@@ -15438,35 +15432,35 @@
       <c r="B489" s="4">
         <v>44408.0</v>
       </c>
-      <c r="C489" s="15">
+      <c r="C489" s="1">
         <v>28217.0</v>
       </c>
       <c r="D489" s="2">
         <f t="shared" si="2"/>
         <v>82</v>
       </c>
-      <c r="E489" s="15">
+      <c r="E489" s="1">
         <v>560.0</v>
       </c>
-      <c r="F489" s="15">
+      <c r="F489" s="1">
         <v>93.0</v>
       </c>
-      <c r="G489" s="15">
+      <c r="G489" s="1">
         <v>92.0</v>
       </c>
-      <c r="H489" s="15">
+      <c r="H489" s="1">
         <v>45.0</v>
       </c>
-      <c r="I489" s="15">
+      <c r="I489" s="1">
         <v>145289.0</v>
       </c>
-      <c r="J489" s="15">
+      <c r="J489" s="1">
         <v>55719.0</v>
       </c>
-      <c r="K489" s="15">
+      <c r="K489" s="1">
         <v>5884.0</v>
       </c>
-      <c r="L489" s="15">
+      <c r="L489" s="1">
         <v>206892.0</v>
       </c>
     </row>
@@ -15478,6 +15472,37 @@
       <c r="B490" s="4">
         <v>44409.0</v>
       </c>
+      <c r="C490" s="15">
+        <v>28271.0</v>
+      </c>
+      <c r="D490" s="2">
+        <f t="shared" si="2"/>
+        <v>54</v>
+      </c>
+      <c r="E490" s="15">
+        <v>560.0</v>
+      </c>
+      <c r="F490" s="15">
+        <v>88.0</v>
+      </c>
+      <c r="G490" s="15">
+        <v>86.0</v>
+      </c>
+      <c r="H490" s="15">
+        <v>47.0</v>
+      </c>
+      <c r="I490" s="15">
+        <v>145325.0</v>
+      </c>
+      <c r="J490" s="15">
+        <v>55885.0</v>
+      </c>
+      <c r="K490" s="15">
+        <v>5884.0</v>
+      </c>
+      <c r="L490" s="15">
+        <v>207094.0</v>
+      </c>
     </row>
     <row r="491" ht="15.75" customHeight="1">
       <c r="A491" s="1">
@@ -15487,6 +15512,37 @@
       <c r="B491" s="4">
         <v>44410.0</v>
       </c>
+      <c r="C491" s="15">
+        <v>28302.0</v>
+      </c>
+      <c r="D491" s="2">
+        <f t="shared" si="2"/>
+        <v>31</v>
+      </c>
+      <c r="E491" s="15">
+        <v>560.0</v>
+      </c>
+      <c r="F491" s="15">
+        <v>93.0</v>
+      </c>
+      <c r="G491" s="15">
+        <v>89.0</v>
+      </c>
+      <c r="H491" s="15">
+        <v>53.0</v>
+      </c>
+      <c r="I491" s="15">
+        <v>145435.0</v>
+      </c>
+      <c r="J491" s="15">
+        <v>55960.0</v>
+      </c>
+      <c r="K491" s="15">
+        <v>5884.0</v>
+      </c>
+      <c r="L491" s="15">
+        <v>207279.0</v>
+      </c>
     </row>
     <row r="492" ht="15.75" customHeight="1">
       <c r="A492" s="1">
@@ -15496,6 +15552,37 @@
       <c r="B492" s="4">
         <v>44411.0</v>
       </c>
+      <c r="C492" s="15">
+        <v>28390.0</v>
+      </c>
+      <c r="D492" s="2">
+        <f t="shared" si="2"/>
+        <v>88</v>
+      </c>
+      <c r="E492" s="15">
+        <v>560.0</v>
+      </c>
+      <c r="F492" s="15">
+        <v>97.0</v>
+      </c>
+      <c r="G492" s="15">
+        <v>92.0</v>
+      </c>
+      <c r="H492" s="15">
+        <v>54.0</v>
+      </c>
+      <c r="I492" s="15">
+        <v>146911.0</v>
+      </c>
+      <c r="J492" s="15">
+        <v>56636.0</v>
+      </c>
+      <c r="K492" s="15">
+        <v>5884.0</v>
+      </c>
+      <c r="L492" s="15">
+        <v>209431.0</v>
+      </c>
     </row>
     <row r="493" ht="15.75" customHeight="1">
       <c r="A493" s="1">
@@ -15505,6 +15592,16 @@
       <c r="B493" s="4">
         <v>44412.0</v>
       </c>
+      <c r="C493" s="2"/>
+      <c r="D493" s="2"/>
+      <c r="E493" s="2"/>
+      <c r="F493" s="2"/>
+      <c r="G493" s="2"/>
+      <c r="H493" s="2"/>
+      <c r="I493" s="2"/>
+      <c r="J493" s="2"/>
+      <c r="K493" s="2"/>
+      <c r="L493" s="2"/>
     </row>
     <row r="494" ht="15.75" customHeight="1">
       <c r="A494" s="1">
@@ -15514,6 +15611,16 @@
       <c r="B494" s="4">
         <v>44413.0</v>
       </c>
+      <c r="C494" s="2"/>
+      <c r="D494" s="2"/>
+      <c r="E494" s="2"/>
+      <c r="F494" s="2"/>
+      <c r="G494" s="2"/>
+      <c r="H494" s="2"/>
+      <c r="I494" s="2"/>
+      <c r="J494" s="2"/>
+      <c r="K494" s="2"/>
+      <c r="L494" s="2"/>
     </row>
     <row r="495" ht="15.75" customHeight="1">
       <c r="A495" s="1">
@@ -15523,6 +15630,16 @@
       <c r="B495" s="4">
         <v>44414.0</v>
       </c>
+      <c r="C495" s="2"/>
+      <c r="D495" s="2"/>
+      <c r="E495" s="2"/>
+      <c r="F495" s="2"/>
+      <c r="G495" s="2"/>
+      <c r="H495" s="2"/>
+      <c r="I495" s="2"/>
+      <c r="J495" s="2"/>
+      <c r="K495" s="2"/>
+      <c r="L495" s="2"/>
     </row>
     <row r="496" ht="15.75" customHeight="1">
       <c r="A496" s="1">
@@ -15532,6 +15649,16 @@
       <c r="B496" s="4">
         <v>44415.0</v>
       </c>
+      <c r="C496" s="2"/>
+      <c r="D496" s="2"/>
+      <c r="E496" s="2"/>
+      <c r="F496" s="2"/>
+      <c r="G496" s="2"/>
+      <c r="H496" s="2"/>
+      <c r="I496" s="2"/>
+      <c r="J496" s="2"/>
+      <c r="K496" s="2"/>
+      <c r="L496" s="2"/>
     </row>
     <row r="497" ht="15.75" customHeight="1">
       <c r="A497" s="1">
@@ -15541,6 +15668,16 @@
       <c r="B497" s="4">
         <v>44416.0</v>
       </c>
+      <c r="C497" s="2"/>
+      <c r="D497" s="2"/>
+      <c r="E497" s="2"/>
+      <c r="F497" s="2"/>
+      <c r="G497" s="2"/>
+      <c r="H497" s="2"/>
+      <c r="I497" s="2"/>
+      <c r="J497" s="2"/>
+      <c r="K497" s="2"/>
+      <c r="L497" s="2"/>
     </row>
     <row r="498" ht="15.75" customHeight="1">
       <c r="A498" s="1">
@@ -15550,6 +15687,16 @@
       <c r="B498" s="4">
         <v>44417.0</v>
       </c>
+      <c r="C498" s="2"/>
+      <c r="D498" s="2"/>
+      <c r="E498" s="2"/>
+      <c r="F498" s="2"/>
+      <c r="G498" s="2"/>
+      <c r="H498" s="2"/>
+      <c r="I498" s="2"/>
+      <c r="J498" s="2"/>
+      <c r="K498" s="2"/>
+      <c r="L498" s="2"/>
     </row>
     <row r="499" ht="15.75" customHeight="1">
       <c r="A499" s="1">
@@ -15559,6 +15706,16 @@
       <c r="B499" s="4">
         <v>44418.0</v>
       </c>
+      <c r="C499" s="2"/>
+      <c r="D499" s="2"/>
+      <c r="E499" s="2"/>
+      <c r="F499" s="2"/>
+      <c r="G499" s="2"/>
+      <c r="H499" s="2"/>
+      <c r="I499" s="2"/>
+      <c r="J499" s="2"/>
+      <c r="K499" s="2"/>
+      <c r="L499" s="2"/>
     </row>
     <row r="500" ht="15.75" customHeight="1">
       <c r="A500" s="1">
@@ -15568,6 +15725,16 @@
       <c r="B500" s="4">
         <v>44419.0</v>
       </c>
+      <c r="C500" s="2"/>
+      <c r="D500" s="2"/>
+      <c r="E500" s="2"/>
+      <c r="F500" s="2"/>
+      <c r="G500" s="2"/>
+      <c r="H500" s="2"/>
+      <c r="I500" s="2"/>
+      <c r="J500" s="2"/>
+      <c r="K500" s="2"/>
+      <c r="L500" s="2"/>
     </row>
     <row r="501" ht="15.75" customHeight="1">
       <c r="A501" s="1">
@@ -15577,6 +15744,16 @@
       <c r="B501" s="4">
         <v>44420.0</v>
       </c>
+      <c r="C501" s="2"/>
+      <c r="D501" s="2"/>
+      <c r="E501" s="2"/>
+      <c r="F501" s="2"/>
+      <c r="G501" s="2"/>
+      <c r="H501" s="2"/>
+      <c r="I501" s="2"/>
+      <c r="J501" s="2"/>
+      <c r="K501" s="2"/>
+      <c r="L501" s="2"/>
     </row>
     <row r="502" ht="15.75" customHeight="1">
       <c r="A502" s="1">
@@ -15586,6 +15763,16 @@
       <c r="B502" s="4">
         <v>44421.0</v>
       </c>
+      <c r="C502" s="2"/>
+      <c r="D502" s="2"/>
+      <c r="E502" s="2"/>
+      <c r="F502" s="2"/>
+      <c r="G502" s="2"/>
+      <c r="H502" s="2"/>
+      <c r="I502" s="2"/>
+      <c r="J502" s="2"/>
+      <c r="K502" s="2"/>
+      <c r="L502" s="2"/>
     </row>
     <row r="503" ht="15.75" customHeight="1">
       <c r="A503" s="1">
@@ -15595,6 +15782,16 @@
       <c r="B503" s="4">
         <v>44422.0</v>
       </c>
+      <c r="C503" s="2"/>
+      <c r="D503" s="2"/>
+      <c r="E503" s="2"/>
+      <c r="F503" s="2"/>
+      <c r="G503" s="2"/>
+      <c r="H503" s="2"/>
+      <c r="I503" s="2"/>
+      <c r="J503" s="2"/>
+      <c r="K503" s="2"/>
+      <c r="L503" s="2"/>
     </row>
     <row r="504" ht="15.75" customHeight="1">
       <c r="A504" s="1">
@@ -15604,6 +15801,16 @@
       <c r="B504" s="4">
         <v>44423.0</v>
       </c>
+      <c r="C504" s="2"/>
+      <c r="D504" s="2"/>
+      <c r="E504" s="2"/>
+      <c r="F504" s="2"/>
+      <c r="G504" s="2"/>
+      <c r="H504" s="2"/>
+      <c r="I504" s="2"/>
+      <c r="J504" s="2"/>
+      <c r="K504" s="2"/>
+      <c r="L504" s="2"/>
     </row>
     <row r="505" ht="15.75" customHeight="1">
       <c r="A505" s="1">
@@ -15613,6 +15820,16 @@
       <c r="B505" s="4">
         <v>44424.0</v>
       </c>
+      <c r="C505" s="2"/>
+      <c r="D505" s="2"/>
+      <c r="E505" s="2"/>
+      <c r="F505" s="2"/>
+      <c r="G505" s="2"/>
+      <c r="H505" s="2"/>
+      <c r="I505" s="2"/>
+      <c r="J505" s="2"/>
+      <c r="K505" s="2"/>
+      <c r="L505" s="2"/>
     </row>
     <row r="506" ht="15.75" customHeight="1">
       <c r="A506" s="1">
@@ -15622,6 +15839,16 @@
       <c r="B506" s="4">
         <v>44425.0</v>
       </c>
+      <c r="C506" s="2"/>
+      <c r="D506" s="2"/>
+      <c r="E506" s="2"/>
+      <c r="F506" s="2"/>
+      <c r="G506" s="2"/>
+      <c r="H506" s="2"/>
+      <c r="I506" s="2"/>
+      <c r="J506" s="2"/>
+      <c r="K506" s="2"/>
+      <c r="L506" s="2"/>
     </row>
     <row r="507" ht="15.75" customHeight="1">
       <c r="A507" s="1">
@@ -15631,6 +15858,16 @@
       <c r="B507" s="4">
         <v>44426.0</v>
       </c>
+      <c r="C507" s="2"/>
+      <c r="D507" s="2"/>
+      <c r="E507" s="2"/>
+      <c r="F507" s="2"/>
+      <c r="G507" s="2"/>
+      <c r="H507" s="2"/>
+      <c r="I507" s="2"/>
+      <c r="J507" s="2"/>
+      <c r="K507" s="2"/>
+      <c r="L507" s="2"/>
     </row>
     <row r="508" ht="15.75" customHeight="1">
       <c r="A508" s="1">
@@ -15640,6 +15877,16 @@
       <c r="B508" s="4">
         <v>44427.0</v>
       </c>
+      <c r="C508" s="2"/>
+      <c r="D508" s="2"/>
+      <c r="E508" s="2"/>
+      <c r="F508" s="2"/>
+      <c r="G508" s="2"/>
+      <c r="H508" s="2"/>
+      <c r="I508" s="2"/>
+      <c r="J508" s="2"/>
+      <c r="K508" s="2"/>
+      <c r="L508" s="2"/>
     </row>
     <row r="509" ht="15.75" customHeight="1">
       <c r="A509" s="1">
@@ -15649,6 +15896,16 @@
       <c r="B509" s="4">
         <v>44428.0</v>
       </c>
+      <c r="C509" s="2"/>
+      <c r="D509" s="2"/>
+      <c r="E509" s="2"/>
+      <c r="F509" s="2"/>
+      <c r="G509" s="2"/>
+      <c r="H509" s="2"/>
+      <c r="I509" s="2"/>
+      <c r="J509" s="2"/>
+      <c r="K509" s="2"/>
+      <c r="L509" s="2"/>
     </row>
     <row r="510" ht="15.75" customHeight="1">
       <c r="A510" s="1">
@@ -15658,6 +15915,16 @@
       <c r="B510" s="4">
         <v>44429.0</v>
       </c>
+      <c r="C510" s="2"/>
+      <c r="D510" s="2"/>
+      <c r="E510" s="2"/>
+      <c r="F510" s="2"/>
+      <c r="G510" s="2"/>
+      <c r="H510" s="2"/>
+      <c r="I510" s="2"/>
+      <c r="J510" s="2"/>
+      <c r="K510" s="2"/>
+      <c r="L510" s="2"/>
     </row>
     <row r="511" ht="15.75" customHeight="1">
       <c r="A511" s="1">
@@ -15667,6 +15934,16 @@
       <c r="B511" s="4">
         <v>44430.0</v>
       </c>
+      <c r="C511" s="2"/>
+      <c r="D511" s="2"/>
+      <c r="E511" s="2"/>
+      <c r="F511" s="2"/>
+      <c r="G511" s="2"/>
+      <c r="H511" s="2"/>
+      <c r="I511" s="2"/>
+      <c r="J511" s="2"/>
+      <c r="K511" s="2"/>
+      <c r="L511" s="2"/>
     </row>
     <row r="512" ht="15.75" customHeight="1">
       <c r="A512" s="1">
@@ -15676,6 +15953,16 @@
       <c r="B512" s="4">
         <v>44431.0</v>
       </c>
+      <c r="C512" s="2"/>
+      <c r="D512" s="2"/>
+      <c r="E512" s="2"/>
+      <c r="F512" s="2"/>
+      <c r="G512" s="2"/>
+      <c r="H512" s="2"/>
+      <c r="I512" s="2"/>
+      <c r="J512" s="2"/>
+      <c r="K512" s="2"/>
+      <c r="L512" s="2"/>
     </row>
     <row r="513" ht="15.75" customHeight="1">
       <c r="A513" s="1">
@@ -15685,6 +15972,16 @@
       <c r="B513" s="4">
         <v>44432.0</v>
       </c>
+      <c r="C513" s="2"/>
+      <c r="D513" s="2"/>
+      <c r="E513" s="2"/>
+      <c r="F513" s="2"/>
+      <c r="G513" s="2"/>
+      <c r="H513" s="2"/>
+      <c r="I513" s="2"/>
+      <c r="J513" s="2"/>
+      <c r="K513" s="2"/>
+      <c r="L513" s="2"/>
     </row>
     <row r="514" ht="15.75" customHeight="1">
       <c r="A514" s="1">
@@ -15694,6 +15991,16 @@
       <c r="B514" s="4">
         <v>44433.0</v>
       </c>
+      <c r="C514" s="2"/>
+      <c r="D514" s="2"/>
+      <c r="E514" s="2"/>
+      <c r="F514" s="2"/>
+      <c r="G514" s="2"/>
+      <c r="H514" s="2"/>
+      <c r="I514" s="2"/>
+      <c r="J514" s="2"/>
+      <c r="K514" s="2"/>
+      <c r="L514" s="2"/>
     </row>
     <row r="515" ht="15.75" customHeight="1">
       <c r="A515" s="1">
@@ -15703,6 +16010,16 @@
       <c r="B515" s="4">
         <v>44434.0</v>
       </c>
+      <c r="C515" s="2"/>
+      <c r="D515" s="2"/>
+      <c r="E515" s="2"/>
+      <c r="F515" s="2"/>
+      <c r="G515" s="2"/>
+      <c r="H515" s="2"/>
+      <c r="I515" s="2"/>
+      <c r="J515" s="2"/>
+      <c r="K515" s="2"/>
+      <c r="L515" s="2"/>
     </row>
     <row r="516" ht="15.75" customHeight="1">
       <c r="A516" s="1">
@@ -15712,6 +16029,16 @@
       <c r="B516" s="4">
         <v>44435.0</v>
       </c>
+      <c r="C516" s="2"/>
+      <c r="D516" s="2"/>
+      <c r="E516" s="2"/>
+      <c r="F516" s="2"/>
+      <c r="G516" s="2"/>
+      <c r="H516" s="2"/>
+      <c r="I516" s="2"/>
+      <c r="J516" s="2"/>
+      <c r="K516" s="2"/>
+      <c r="L516" s="2"/>
     </row>
     <row r="517" ht="15.75" customHeight="1">
       <c r="A517" s="1">
@@ -15721,6 +16048,16 @@
       <c r="B517" s="4">
         <v>44436.0</v>
       </c>
+      <c r="C517" s="2"/>
+      <c r="D517" s="2"/>
+      <c r="E517" s="2"/>
+      <c r="F517" s="2"/>
+      <c r="G517" s="2"/>
+      <c r="H517" s="2"/>
+      <c r="I517" s="2"/>
+      <c r="J517" s="2"/>
+      <c r="K517" s="2"/>
+      <c r="L517" s="2"/>
     </row>
     <row r="518" ht="15.75" customHeight="1">
       <c r="A518" s="1">
@@ -15730,6 +16067,16 @@
       <c r="B518" s="4">
         <v>44437.0</v>
       </c>
+      <c r="C518" s="2"/>
+      <c r="D518" s="2"/>
+      <c r="E518" s="2"/>
+      <c r="F518" s="2"/>
+      <c r="G518" s="2"/>
+      <c r="H518" s="2"/>
+      <c r="I518" s="2"/>
+      <c r="J518" s="2"/>
+      <c r="K518" s="2"/>
+      <c r="L518" s="2"/>
     </row>
     <row r="519" ht="15.75" customHeight="1">
       <c r="A519" s="1">
@@ -15739,6 +16086,16 @@
       <c r="B519" s="4">
         <v>44438.0</v>
       </c>
+      <c r="C519" s="2"/>
+      <c r="D519" s="2"/>
+      <c r="E519" s="2"/>
+      <c r="F519" s="2"/>
+      <c r="G519" s="2"/>
+      <c r="H519" s="2"/>
+      <c r="I519" s="2"/>
+      <c r="J519" s="2"/>
+      <c r="K519" s="2"/>
+      <c r="L519" s="2"/>
     </row>
     <row r="520" ht="15.75" customHeight="1">
       <c r="A520" s="1">
@@ -15748,9 +16105,19 @@
       <c r="B520" s="4">
         <v>44439.0</v>
       </c>
+      <c r="C520" s="2"/>
+      <c r="D520" s="2"/>
+      <c r="E520" s="2"/>
+      <c r="F520" s="2"/>
+      <c r="G520" s="2"/>
+      <c r="H520" s="2"/>
+      <c r="I520" s="2"/>
+      <c r="J520" s="2"/>
+      <c r="K520" s="2"/>
+      <c r="L520" s="2"/>
     </row>
     <row r="521" ht="15.75" customHeight="1">
-      <c r="B521" s="17"/>
+      <c r="B521" s="4"/>
     </row>
     <row r="522" ht="15.75" customHeight="1"/>
     <row r="523" ht="15.75" customHeight="1"/>
@@ -16233,7 +16600,7 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{8C5E459B-F781-4902-BF57-DF5AFCFB730D}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{35B53A02-2CED-4375-A753-341DF5F2FA7E}" filter="1" showAutoFilter="1">
       <autoFilter ref="$G$9"/>
       <extLst>
         <ext uri="GoogleSheetsCustomDataVersion1">

</xml_diff>

<commit_message>
Added data on 7 Aug
</commit_message>
<xml_diff>
--- a/Araraquara_covid.xlsx
+++ b/Araraquara_covid.xlsx
@@ -6,11 +6,11 @@
     <sheet state="visible" name="Araraquara covid.csv" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="Z_35B53A02_2CED_4375_A753_341DF5F2FA7E_.wvu.FilterData">'Araraquara covid.csv'!$G$9</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_1B7F48FD_B353_4FFD_A0DA_E3D5BAFE3953_.wvu.FilterData">'Araraquara covid.csv'!$G$9</definedName>
   </definedNames>
   <calcPr/>
   <customWorkbookViews>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{35B53A02-2CED-4375-A753-341DF5F2FA7E}" name="Filtro 1"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{1B7F48FD-B353-4FFD-A0DA-E3D5BAFE3953}" name="Filtro 1"/>
   </customWorkbookViews>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
@@ -568,7 +568,7 @@
         <v>5.0</v>
       </c>
       <c r="D3" s="2">
-        <f t="shared" ref="D3:D492" si="2">(C3-C2)</f>
+        <f t="shared" ref="D3:D496" si="2">(C3-C2)</f>
         <v>2</v>
       </c>
       <c r="E3" s="1">
@@ -15472,35 +15472,35 @@
       <c r="B490" s="4">
         <v>44409.0</v>
       </c>
-      <c r="C490" s="15">
+      <c r="C490" s="1">
         <v>28271.0</v>
       </c>
       <c r="D490" s="2">
         <f t="shared" si="2"/>
         <v>54</v>
       </c>
-      <c r="E490" s="15">
+      <c r="E490" s="1">
         <v>560.0</v>
       </c>
-      <c r="F490" s="15">
+      <c r="F490" s="1">
         <v>88.0</v>
       </c>
-      <c r="G490" s="15">
+      <c r="G490" s="1">
         <v>86.0</v>
       </c>
-      <c r="H490" s="15">
+      <c r="H490" s="1">
         <v>47.0</v>
       </c>
-      <c r="I490" s="15">
+      <c r="I490" s="1">
         <v>145325.0</v>
       </c>
-      <c r="J490" s="15">
+      <c r="J490" s="1">
         <v>55885.0</v>
       </c>
-      <c r="K490" s="15">
+      <c r="K490" s="1">
         <v>5884.0</v>
       </c>
-      <c r="L490" s="15">
+      <c r="L490" s="1">
         <v>207094.0</v>
       </c>
     </row>
@@ -15512,35 +15512,35 @@
       <c r="B491" s="4">
         <v>44410.0</v>
       </c>
-      <c r="C491" s="15">
+      <c r="C491" s="1">
         <v>28302.0</v>
       </c>
       <c r="D491" s="2">
         <f t="shared" si="2"/>
         <v>31</v>
       </c>
-      <c r="E491" s="15">
+      <c r="E491" s="1">
         <v>560.0</v>
       </c>
-      <c r="F491" s="15">
+      <c r="F491" s="1">
         <v>93.0</v>
       </c>
-      <c r="G491" s="15">
+      <c r="G491" s="1">
         <v>89.0</v>
       </c>
-      <c r="H491" s="15">
+      <c r="H491" s="1">
         <v>53.0</v>
       </c>
-      <c r="I491" s="15">
+      <c r="I491" s="1">
         <v>145435.0</v>
       </c>
-      <c r="J491" s="15">
+      <c r="J491" s="1">
         <v>55960.0</v>
       </c>
-      <c r="K491" s="15">
+      <c r="K491" s="1">
         <v>5884.0</v>
       </c>
-      <c r="L491" s="15">
+      <c r="L491" s="1">
         <v>207279.0</v>
       </c>
     </row>
@@ -15552,35 +15552,35 @@
       <c r="B492" s="4">
         <v>44411.0</v>
       </c>
-      <c r="C492" s="15">
+      <c r="C492" s="1">
         <v>28390.0</v>
       </c>
       <c r="D492" s="2">
         <f t="shared" si="2"/>
         <v>88</v>
       </c>
-      <c r="E492" s="15">
+      <c r="E492" s="1">
         <v>560.0</v>
       </c>
-      <c r="F492" s="15">
+      <c r="F492" s="1">
         <v>97.0</v>
       </c>
-      <c r="G492" s="15">
+      <c r="G492" s="1">
         <v>92.0</v>
       </c>
-      <c r="H492" s="15">
+      <c r="H492" s="1">
         <v>54.0</v>
       </c>
-      <c r="I492" s="15">
+      <c r="I492" s="1">
         <v>146911.0</v>
       </c>
-      <c r="J492" s="15">
+      <c r="J492" s="1">
         <v>56636.0</v>
       </c>
-      <c r="K492" s="15">
+      <c r="K492" s="1">
         <v>5884.0</v>
       </c>
-      <c r="L492" s="15">
+      <c r="L492" s="1">
         <v>209431.0</v>
       </c>
     </row>
@@ -15592,16 +15592,37 @@
       <c r="B493" s="4">
         <v>44412.0</v>
       </c>
-      <c r="C493" s="2"/>
-      <c r="D493" s="2"/>
-      <c r="E493" s="2"/>
-      <c r="F493" s="2"/>
-      <c r="G493" s="2"/>
-      <c r="H493" s="2"/>
-      <c r="I493" s="2"/>
-      <c r="J493" s="2"/>
-      <c r="K493" s="2"/>
-      <c r="L493" s="2"/>
+      <c r="C493" s="15">
+        <v>28464.0</v>
+      </c>
+      <c r="D493" s="2">
+        <f t="shared" si="2"/>
+        <v>74</v>
+      </c>
+      <c r="E493" s="15">
+        <v>562.0</v>
+      </c>
+      <c r="F493" s="15">
+        <v>93.0</v>
+      </c>
+      <c r="G493" s="15">
+        <v>89.0</v>
+      </c>
+      <c r="H493" s="15">
+        <v>44.0</v>
+      </c>
+      <c r="I493" s="15">
+        <v>149376.0</v>
+      </c>
+      <c r="J493" s="15">
+        <v>57776.0</v>
+      </c>
+      <c r="K493" s="15">
+        <v>5902.0</v>
+      </c>
+      <c r="L493" s="15">
+        <v>213054.0</v>
+      </c>
     </row>
     <row r="494" ht="15.75" customHeight="1">
       <c r="A494" s="1">
@@ -15611,16 +15632,37 @@
       <c r="B494" s="4">
         <v>44413.0</v>
       </c>
-      <c r="C494" s="2"/>
-      <c r="D494" s="2"/>
-      <c r="E494" s="2"/>
-      <c r="F494" s="2"/>
-      <c r="G494" s="2"/>
-      <c r="H494" s="2"/>
-      <c r="I494" s="2"/>
-      <c r="J494" s="2"/>
-      <c r="K494" s="2"/>
-      <c r="L494" s="2"/>
+      <c r="C494" s="15">
+        <v>28535.0</v>
+      </c>
+      <c r="D494" s="2">
+        <f t="shared" si="2"/>
+        <v>71</v>
+      </c>
+      <c r="E494" s="15">
+        <v>563.0</v>
+      </c>
+      <c r="F494" s="15">
+        <v>87.0</v>
+      </c>
+      <c r="G494" s="15">
+        <v>83.0</v>
+      </c>
+      <c r="H494" s="15">
+        <v>46.0</v>
+      </c>
+      <c r="I494" s="15">
+        <v>151641.0</v>
+      </c>
+      <c r="J494" s="15">
+        <v>58547.0</v>
+      </c>
+      <c r="K494" s="15">
+        <v>5941.0</v>
+      </c>
+      <c r="L494" s="15">
+        <v>216129.0</v>
+      </c>
     </row>
     <row r="495" ht="15.75" customHeight="1">
       <c r="A495" s="1">
@@ -15630,16 +15672,37 @@
       <c r="B495" s="4">
         <v>44414.0</v>
       </c>
-      <c r="C495" s="2"/>
-      <c r="D495" s="2"/>
-      <c r="E495" s="2"/>
-      <c r="F495" s="2"/>
-      <c r="G495" s="2"/>
-      <c r="H495" s="2"/>
-      <c r="I495" s="2"/>
-      <c r="J495" s="2"/>
-      <c r="K495" s="2"/>
-      <c r="L495" s="2"/>
+      <c r="C495" s="15">
+        <v>28599.0</v>
+      </c>
+      <c r="D495" s="2">
+        <f t="shared" si="2"/>
+        <v>64</v>
+      </c>
+      <c r="E495" s="15">
+        <v>563.0</v>
+      </c>
+      <c r="F495" s="15">
+        <v>80.0</v>
+      </c>
+      <c r="G495" s="15">
+        <v>77.0</v>
+      </c>
+      <c r="H495" s="15">
+        <v>42.0</v>
+      </c>
+      <c r="I495" s="15">
+        <v>153463.0</v>
+      </c>
+      <c r="J495" s="15">
+        <v>59261.0</v>
+      </c>
+      <c r="K495" s="15">
+        <v>5941.0</v>
+      </c>
+      <c r="L495" s="15">
+        <v>218665.0</v>
+      </c>
     </row>
     <row r="496" ht="15.75" customHeight="1">
       <c r="A496" s="1">
@@ -15649,16 +15712,37 @@
       <c r="B496" s="4">
         <v>44415.0</v>
       </c>
-      <c r="C496" s="2"/>
-      <c r="D496" s="2"/>
-      <c r="E496" s="2"/>
-      <c r="F496" s="2"/>
-      <c r="G496" s="2"/>
-      <c r="H496" s="2"/>
-      <c r="I496" s="2"/>
-      <c r="J496" s="2"/>
-      <c r="K496" s="2"/>
-      <c r="L496" s="2"/>
+      <c r="C496" s="15">
+        <v>28666.0</v>
+      </c>
+      <c r="D496" s="2">
+        <f t="shared" si="2"/>
+        <v>67</v>
+      </c>
+      <c r="E496" s="15">
+        <v>563.0</v>
+      </c>
+      <c r="F496" s="15">
+        <v>72.0</v>
+      </c>
+      <c r="G496" s="15">
+        <v>70.0</v>
+      </c>
+      <c r="H496" s="15">
+        <v>45.0</v>
+      </c>
+      <c r="I496" s="15">
+        <v>155437.0</v>
+      </c>
+      <c r="J496" s="15">
+        <v>60118.0</v>
+      </c>
+      <c r="K496" s="15">
+        <v>5941.0</v>
+      </c>
+      <c r="L496" s="15">
+        <v>221496.0</v>
+      </c>
     </row>
     <row r="497" ht="15.75" customHeight="1">
       <c r="A497" s="1">
@@ -16600,7 +16684,7 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{35B53A02-2CED-4375-A753-341DF5F2FA7E}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{1B7F48FD-B353-4FFD-A0DA-E3D5BAFE3953}" filter="1" showAutoFilter="1">
       <autoFilter ref="$G$9"/>
       <extLst>
         <ext uri="GoogleSheetsCustomDataVersion1">

</xml_diff>

<commit_message>
Added data on 14 Aug
</commit_message>
<xml_diff>
--- a/Araraquara_covid.xlsx
+++ b/Araraquara_covid.xlsx
@@ -6,11 +6,11 @@
     <sheet state="visible" name="Araraquara covid.csv" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="Z_1B7F48FD_B353_4FFD_A0DA_E3D5BAFE3953_.wvu.FilterData">'Araraquara covid.csv'!$G$9</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_12621F90_3527_4EC5_8665_E3613A458E47_.wvu.FilterData">'Araraquara covid.csv'!$G$9</definedName>
   </definedNames>
   <calcPr/>
   <customWorkbookViews>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{1B7F48FD-B353-4FFD-A0DA-E3D5BAFE3953}" name="Filtro 1"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{12621F90-3527-4EC5-8665-E3613A458E47}" name="Filtro 1"/>
   </customWorkbookViews>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
@@ -568,7 +568,7 @@
         <v>5.0</v>
       </c>
       <c r="D3" s="2">
-        <f t="shared" ref="D3:D496" si="2">(C3-C2)</f>
+        <f t="shared" ref="D3:D503" si="2">(C3-C2)</f>
         <v>2</v>
       </c>
       <c r="E3" s="1">
@@ -15592,35 +15592,35 @@
       <c r="B493" s="4">
         <v>44412.0</v>
       </c>
-      <c r="C493" s="15">
+      <c r="C493" s="1">
         <v>28464.0</v>
       </c>
       <c r="D493" s="2">
         <f t="shared" si="2"/>
         <v>74</v>
       </c>
-      <c r="E493" s="15">
+      <c r="E493" s="1">
         <v>562.0</v>
       </c>
-      <c r="F493" s="15">
+      <c r="F493" s="1">
         <v>93.0</v>
       </c>
-      <c r="G493" s="15">
+      <c r="G493" s="1">
         <v>89.0</v>
       </c>
-      <c r="H493" s="15">
+      <c r="H493" s="1">
         <v>44.0</v>
       </c>
-      <c r="I493" s="15">
+      <c r="I493" s="1">
         <v>149376.0</v>
       </c>
-      <c r="J493" s="15">
+      <c r="J493" s="1">
         <v>57776.0</v>
       </c>
-      <c r="K493" s="15">
+      <c r="K493" s="1">
         <v>5902.0</v>
       </c>
-      <c r="L493" s="15">
+      <c r="L493" s="1">
         <v>213054.0</v>
       </c>
     </row>
@@ -15632,35 +15632,35 @@
       <c r="B494" s="4">
         <v>44413.0</v>
       </c>
-      <c r="C494" s="15">
+      <c r="C494" s="1">
         <v>28535.0</v>
       </c>
       <c r="D494" s="2">
         <f t="shared" si="2"/>
         <v>71</v>
       </c>
-      <c r="E494" s="15">
+      <c r="E494" s="1">
         <v>563.0</v>
       </c>
-      <c r="F494" s="15">
+      <c r="F494" s="1">
         <v>87.0</v>
       </c>
-      <c r="G494" s="15">
+      <c r="G494" s="1">
         <v>83.0</v>
       </c>
-      <c r="H494" s="15">
+      <c r="H494" s="1">
         <v>46.0</v>
       </c>
-      <c r="I494" s="15">
+      <c r="I494" s="1">
         <v>151641.0</v>
       </c>
-      <c r="J494" s="15">
+      <c r="J494" s="1">
         <v>58547.0</v>
       </c>
-      <c r="K494" s="15">
+      <c r="K494" s="1">
         <v>5941.0</v>
       </c>
-      <c r="L494" s="15">
+      <c r="L494" s="1">
         <v>216129.0</v>
       </c>
     </row>
@@ -15672,35 +15672,35 @@
       <c r="B495" s="4">
         <v>44414.0</v>
       </c>
-      <c r="C495" s="15">
+      <c r="C495" s="1">
         <v>28599.0</v>
       </c>
       <c r="D495" s="2">
         <f t="shared" si="2"/>
         <v>64</v>
       </c>
-      <c r="E495" s="15">
+      <c r="E495" s="1">
         <v>563.0</v>
       </c>
-      <c r="F495" s="15">
+      <c r="F495" s="1">
         <v>80.0</v>
       </c>
-      <c r="G495" s="15">
+      <c r="G495" s="1">
         <v>77.0</v>
       </c>
-      <c r="H495" s="15">
+      <c r="H495" s="1">
         <v>42.0</v>
       </c>
-      <c r="I495" s="15">
+      <c r="I495" s="1">
         <v>153463.0</v>
       </c>
-      <c r="J495" s="15">
+      <c r="J495" s="1">
         <v>59261.0</v>
       </c>
-      <c r="K495" s="15">
+      <c r="K495" s="1">
         <v>5941.0</v>
       </c>
-      <c r="L495" s="15">
+      <c r="L495" s="1">
         <v>218665.0</v>
       </c>
     </row>
@@ -15712,35 +15712,35 @@
       <c r="B496" s="4">
         <v>44415.0</v>
       </c>
-      <c r="C496" s="15">
+      <c r="C496" s="1">
         <v>28666.0</v>
       </c>
       <c r="D496" s="2">
         <f t="shared" si="2"/>
         <v>67</v>
       </c>
-      <c r="E496" s="15">
+      <c r="E496" s="1">
         <v>563.0</v>
       </c>
-      <c r="F496" s="15">
+      <c r="F496" s="1">
         <v>72.0</v>
       </c>
-      <c r="G496" s="15">
+      <c r="G496" s="1">
         <v>70.0</v>
       </c>
-      <c r="H496" s="15">
+      <c r="H496" s="1">
         <v>45.0</v>
       </c>
-      <c r="I496" s="15">
+      <c r="I496" s="1">
         <v>155437.0</v>
       </c>
-      <c r="J496" s="15">
+      <c r="J496" s="1">
         <v>60118.0</v>
       </c>
-      <c r="K496" s="15">
+      <c r="K496" s="1">
         <v>5941.0</v>
       </c>
-      <c r="L496" s="15">
+      <c r="L496" s="1">
         <v>221496.0</v>
       </c>
     </row>
@@ -15752,16 +15752,37 @@
       <c r="B497" s="4">
         <v>44416.0</v>
       </c>
-      <c r="C497" s="2"/>
-      <c r="D497" s="2"/>
-      <c r="E497" s="2"/>
-      <c r="F497" s="2"/>
-      <c r="G497" s="2"/>
-      <c r="H497" s="2"/>
-      <c r="I497" s="2"/>
-      <c r="J497" s="2"/>
-      <c r="K497" s="2"/>
-      <c r="L497" s="2"/>
+      <c r="C497" s="1">
+        <v>28716.0</v>
+      </c>
+      <c r="D497" s="2">
+        <f t="shared" si="2"/>
+        <v>50</v>
+      </c>
+      <c r="E497" s="1">
+        <v>563.0</v>
+      </c>
+      <c r="F497" s="1">
+        <v>65.0</v>
+      </c>
+      <c r="G497" s="1">
+        <v>64.0</v>
+      </c>
+      <c r="H497" s="1">
+        <v>40.0</v>
+      </c>
+      <c r="I497" s="1">
+        <v>155901.0</v>
+      </c>
+      <c r="J497" s="1">
+        <v>60262.0</v>
+      </c>
+      <c r="K497" s="1">
+        <v>5941.0</v>
+      </c>
+      <c r="L497" s="1">
+        <v>222104.0</v>
+      </c>
     </row>
     <row r="498" ht="15.75" customHeight="1">
       <c r="A498" s="1">
@@ -15771,16 +15792,37 @@
       <c r="B498" s="4">
         <v>44417.0</v>
       </c>
-      <c r="C498" s="2"/>
-      <c r="D498" s="2"/>
-      <c r="E498" s="2"/>
-      <c r="F498" s="2"/>
-      <c r="G498" s="2"/>
-      <c r="H498" s="2"/>
-      <c r="I498" s="2"/>
-      <c r="J498" s="2"/>
-      <c r="K498" s="2"/>
-      <c r="L498" s="2"/>
+      <c r="C498" s="1">
+        <v>28730.0</v>
+      </c>
+      <c r="D498" s="2">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="E498" s="1">
+        <v>564.0</v>
+      </c>
+      <c r="F498" s="1">
+        <v>61.0</v>
+      </c>
+      <c r="G498" s="1">
+        <v>59.0</v>
+      </c>
+      <c r="H498" s="1">
+        <v>39.0</v>
+      </c>
+      <c r="I498" s="1">
+        <v>156053.0</v>
+      </c>
+      <c r="J498" s="1">
+        <v>60289.0</v>
+      </c>
+      <c r="K498" s="1">
+        <v>5941.0</v>
+      </c>
+      <c r="L498" s="1">
+        <v>222283.0</v>
+      </c>
     </row>
     <row r="499" ht="15.75" customHeight="1">
       <c r="A499" s="1">
@@ -15790,16 +15832,37 @@
       <c r="B499" s="4">
         <v>44418.0</v>
       </c>
-      <c r="C499" s="2"/>
-      <c r="D499" s="2"/>
-      <c r="E499" s="2"/>
-      <c r="F499" s="2"/>
-      <c r="G499" s="2"/>
-      <c r="H499" s="2"/>
-      <c r="I499" s="2"/>
-      <c r="J499" s="2"/>
-      <c r="K499" s="2"/>
-      <c r="L499" s="2"/>
+      <c r="C499" s="1">
+        <v>28771.0</v>
+      </c>
+      <c r="D499" s="2">
+        <f t="shared" si="2"/>
+        <v>41</v>
+      </c>
+      <c r="E499" s="1">
+        <v>565.0</v>
+      </c>
+      <c r="F499" s="1">
+        <v>68.0</v>
+      </c>
+      <c r="G499" s="1">
+        <v>65.0</v>
+      </c>
+      <c r="H499" s="1">
+        <v>41.0</v>
+      </c>
+      <c r="I499" s="1">
+        <v>157889.0</v>
+      </c>
+      <c r="J499" s="1">
+        <v>60963.0</v>
+      </c>
+      <c r="K499" s="1">
+        <v>5942.0</v>
+      </c>
+      <c r="L499" s="1">
+        <v>224794.0</v>
+      </c>
     </row>
     <row r="500" ht="15.75" customHeight="1">
       <c r="A500" s="1">
@@ -15809,16 +15872,37 @@
       <c r="B500" s="4">
         <v>44419.0</v>
       </c>
-      <c r="C500" s="2"/>
-      <c r="D500" s="2"/>
-      <c r="E500" s="2"/>
-      <c r="F500" s="2"/>
-      <c r="G500" s="2"/>
-      <c r="H500" s="2"/>
-      <c r="I500" s="2"/>
-      <c r="J500" s="2"/>
-      <c r="K500" s="2"/>
-      <c r="L500" s="2"/>
+      <c r="C500" s="1">
+        <v>28865.0</v>
+      </c>
+      <c r="D500" s="2">
+        <f t="shared" si="2"/>
+        <v>94</v>
+      </c>
+      <c r="E500" s="1">
+        <v>565.0</v>
+      </c>
+      <c r="F500" s="1">
+        <v>62.0</v>
+      </c>
+      <c r="G500" s="1">
+        <v>61.0</v>
+      </c>
+      <c r="H500" s="1">
+        <v>36.0</v>
+      </c>
+      <c r="I500" s="1">
+        <v>158919.0</v>
+      </c>
+      <c r="J500" s="1">
+        <v>61676.0</v>
+      </c>
+      <c r="K500" s="1">
+        <v>5942.0</v>
+      </c>
+      <c r="L500" s="1">
+        <v>226537.0</v>
+      </c>
     </row>
     <row r="501" ht="15.75" customHeight="1">
       <c r="A501" s="1">
@@ -15828,16 +15912,37 @@
       <c r="B501" s="4">
         <v>44420.0</v>
       </c>
-      <c r="C501" s="2"/>
-      <c r="D501" s="2"/>
-      <c r="E501" s="2"/>
-      <c r="F501" s="2"/>
-      <c r="G501" s="2"/>
-      <c r="H501" s="2"/>
-      <c r="I501" s="2"/>
-      <c r="J501" s="2"/>
-      <c r="K501" s="2"/>
-      <c r="L501" s="2"/>
+      <c r="C501" s="1">
+        <v>28904.0</v>
+      </c>
+      <c r="D501" s="2">
+        <f t="shared" si="2"/>
+        <v>39</v>
+      </c>
+      <c r="E501" s="1">
+        <v>566.0</v>
+      </c>
+      <c r="F501" s="1">
+        <v>59.0</v>
+      </c>
+      <c r="G501" s="1">
+        <v>58.0</v>
+      </c>
+      <c r="H501" s="1">
+        <v>32.0</v>
+      </c>
+      <c r="I501" s="1">
+        <v>160557.0</v>
+      </c>
+      <c r="J501" s="1">
+        <v>62633.0</v>
+      </c>
+      <c r="K501" s="1">
+        <v>5943.0</v>
+      </c>
+      <c r="L501" s="1">
+        <v>229133.0</v>
+      </c>
     </row>
     <row r="502" ht="15.75" customHeight="1">
       <c r="A502" s="1">
@@ -15847,16 +15952,37 @@
       <c r="B502" s="4">
         <v>44421.0</v>
       </c>
-      <c r="C502" s="2"/>
-      <c r="D502" s="2"/>
-      <c r="E502" s="2"/>
-      <c r="F502" s="2"/>
-      <c r="G502" s="2"/>
-      <c r="H502" s="2"/>
-      <c r="I502" s="2"/>
-      <c r="J502" s="2"/>
-      <c r="K502" s="2"/>
-      <c r="L502" s="2"/>
+      <c r="C502" s="1">
+        <v>28956.0</v>
+      </c>
+      <c r="D502" s="2">
+        <f t="shared" si="2"/>
+        <v>52</v>
+      </c>
+      <c r="E502" s="1">
+        <v>566.0</v>
+      </c>
+      <c r="F502" s="1">
+        <v>61.0</v>
+      </c>
+      <c r="G502" s="1">
+        <v>60.0</v>
+      </c>
+      <c r="H502" s="1">
+        <v>33.0</v>
+      </c>
+      <c r="I502" s="1">
+        <v>162744.0</v>
+      </c>
+      <c r="J502" s="1">
+        <v>63766.0</v>
+      </c>
+      <c r="K502" s="1">
+        <v>5943.0</v>
+      </c>
+      <c r="L502" s="1">
+        <v>232453.0</v>
+      </c>
     </row>
     <row r="503" ht="15.75" customHeight="1">
       <c r="A503" s="1">
@@ -15866,16 +15992,37 @@
       <c r="B503" s="4">
         <v>44422.0</v>
       </c>
-      <c r="C503" s="2"/>
-      <c r="D503" s="2"/>
-      <c r="E503" s="2"/>
-      <c r="F503" s="2"/>
-      <c r="G503" s="2"/>
-      <c r="H503" s="2"/>
-      <c r="I503" s="2"/>
-      <c r="J503" s="2"/>
-      <c r="K503" s="2"/>
-      <c r="L503" s="2"/>
+      <c r="C503" s="15">
+        <v>28995.0</v>
+      </c>
+      <c r="D503" s="2">
+        <f t="shared" si="2"/>
+        <v>39</v>
+      </c>
+      <c r="E503" s="15">
+        <v>566.0</v>
+      </c>
+      <c r="F503" s="15">
+        <v>58.0</v>
+      </c>
+      <c r="G503" s="15">
+        <v>56.0</v>
+      </c>
+      <c r="H503" s="15">
+        <v>34.0</v>
+      </c>
+      <c r="I503" s="15">
+        <v>165134.0</v>
+      </c>
+      <c r="J503" s="15">
+        <v>64846.0</v>
+      </c>
+      <c r="K503" s="15">
+        <v>6943.0</v>
+      </c>
+      <c r="L503" s="15">
+        <v>235923.0</v>
+      </c>
     </row>
     <row r="504" ht="15.75" customHeight="1">
       <c r="A504" s="1">
@@ -16684,7 +16831,7 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{1B7F48FD-B353-4FFD-A0DA-E3D5BAFE3953}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{12621F90-3527-4EC5-8665-E3613A458E47}" filter="1" showAutoFilter="1">
       <autoFilter ref="$G$9"/>
       <extLst>
         <ext uri="GoogleSheetsCustomDataVersion1">

</xml_diff>

<commit_message>
Added data on 21 Aug
</commit_message>
<xml_diff>
--- a/Araraquara_covid.xlsx
+++ b/Araraquara_covid.xlsx
@@ -6,11 +6,11 @@
     <sheet state="visible" name="Araraquara covid.csv" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="Z_12621F90_3527_4EC5_8665_E3613A458E47_.wvu.FilterData">'Araraquara covid.csv'!$G$9</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_3048ACAE_E4B1_45E5_83C0_B10EF9140B30_.wvu.FilterData">'Araraquara covid.csv'!$G$9</definedName>
   </definedNames>
   <calcPr/>
   <customWorkbookViews>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{12621F90-3527-4EC5-8665-E3613A458E47}" name="Filtro 1"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{3048ACAE-E4B1-45E5-83C0-B10EF9140B30}" name="Filtro 1"/>
   </customWorkbookViews>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
@@ -568,7 +568,7 @@
         <v>5.0</v>
       </c>
       <c r="D3" s="2">
-        <f t="shared" ref="D3:D503" si="2">(C3-C2)</f>
+        <f t="shared" ref="D3:D510" si="2">(C3-C2)</f>
         <v>2</v>
       </c>
       <c r="E3" s="1">
@@ -15992,35 +15992,35 @@
       <c r="B503" s="4">
         <v>44422.0</v>
       </c>
-      <c r="C503" s="15">
+      <c r="C503" s="1">
         <v>28995.0</v>
       </c>
       <c r="D503" s="2">
         <f t="shared" si="2"/>
         <v>39</v>
       </c>
-      <c r="E503" s="15">
+      <c r="E503" s="1">
         <v>566.0</v>
       </c>
-      <c r="F503" s="15">
+      <c r="F503" s="1">
         <v>58.0</v>
       </c>
-      <c r="G503" s="15">
+      <c r="G503" s="1">
         <v>56.0</v>
       </c>
-      <c r="H503" s="15">
+      <c r="H503" s="1">
         <v>34.0</v>
       </c>
-      <c r="I503" s="15">
+      <c r="I503" s="1">
         <v>165134.0</v>
       </c>
-      <c r="J503" s="15">
+      <c r="J503" s="1">
         <v>64846.0</v>
       </c>
-      <c r="K503" s="15">
-        <v>6943.0</v>
-      </c>
-      <c r="L503" s="15">
+      <c r="K503" s="1">
+        <v>5943.0</v>
+      </c>
+      <c r="L503" s="1">
         <v>235923.0</v>
       </c>
     </row>
@@ -16032,16 +16032,37 @@
       <c r="B504" s="4">
         <v>44423.0</v>
       </c>
-      <c r="C504" s="2"/>
-      <c r="D504" s="2"/>
-      <c r="E504" s="2"/>
-      <c r="F504" s="2"/>
-      <c r="G504" s="2"/>
-      <c r="H504" s="2"/>
-      <c r="I504" s="2"/>
-      <c r="J504" s="2"/>
-      <c r="K504" s="2"/>
-      <c r="L504" s="2"/>
+      <c r="C504" s="1">
+        <v>29027.0</v>
+      </c>
+      <c r="D504" s="2">
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
+      <c r="E504" s="1">
+        <v>568.0</v>
+      </c>
+      <c r="F504" s="1">
+        <v>52.0</v>
+      </c>
+      <c r="G504" s="1">
+        <v>51.0</v>
+      </c>
+      <c r="H504" s="1">
+        <v>28.0</v>
+      </c>
+      <c r="I504" s="1">
+        <v>165247.0</v>
+      </c>
+      <c r="J504" s="1">
+        <v>64890.0</v>
+      </c>
+      <c r="K504" s="1">
+        <v>5943.0</v>
+      </c>
+      <c r="L504" s="1">
+        <v>236080.0</v>
+      </c>
     </row>
     <row r="505" ht="15.75" customHeight="1">
       <c r="A505" s="1">
@@ -16051,16 +16072,37 @@
       <c r="B505" s="4">
         <v>44424.0</v>
       </c>
-      <c r="C505" s="2"/>
-      <c r="D505" s="2"/>
-      <c r="E505" s="2"/>
-      <c r="F505" s="2"/>
-      <c r="G505" s="2"/>
-      <c r="H505" s="2"/>
-      <c r="I505" s="2"/>
-      <c r="J505" s="2"/>
-      <c r="K505" s="2"/>
-      <c r="L505" s="2"/>
+      <c r="C505" s="1">
+        <v>29034.0</v>
+      </c>
+      <c r="D505" s="2">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="E505" s="1">
+        <v>569.0</v>
+      </c>
+      <c r="F505" s="1">
+        <v>54.0</v>
+      </c>
+      <c r="G505" s="1">
+        <v>51.0</v>
+      </c>
+      <c r="H505" s="1">
+        <v>27.0</v>
+      </c>
+      <c r="I505" s="1">
+        <v>165300.0</v>
+      </c>
+      <c r="J505" s="1">
+        <v>64950.0</v>
+      </c>
+      <c r="K505" s="1">
+        <v>5943.0</v>
+      </c>
+      <c r="L505" s="1">
+        <v>236193.0</v>
+      </c>
     </row>
     <row r="506" ht="15.75" customHeight="1">
       <c r="A506" s="1">
@@ -16070,16 +16112,37 @@
       <c r="B506" s="4">
         <v>44425.0</v>
       </c>
-      <c r="C506" s="2"/>
-      <c r="D506" s="2"/>
-      <c r="E506" s="2"/>
-      <c r="F506" s="2"/>
-      <c r="G506" s="2"/>
-      <c r="H506" s="2"/>
-      <c r="I506" s="2"/>
-      <c r="J506" s="2"/>
-      <c r="K506" s="2"/>
-      <c r="L506" s="2"/>
+      <c r="C506" s="1">
+        <v>29114.0</v>
+      </c>
+      <c r="D506" s="2">
+        <f t="shared" si="2"/>
+        <v>80</v>
+      </c>
+      <c r="E506" s="1">
+        <v>569.0</v>
+      </c>
+      <c r="F506" s="1">
+        <v>47.0</v>
+      </c>
+      <c r="G506" s="1">
+        <v>46.0</v>
+      </c>
+      <c r="H506" s="1">
+        <v>26.0</v>
+      </c>
+      <c r="I506" s="1">
+        <v>167382.0</v>
+      </c>
+      <c r="J506" s="1">
+        <v>66139.0</v>
+      </c>
+      <c r="K506" s="1">
+        <v>5944.0</v>
+      </c>
+      <c r="L506" s="1">
+        <v>239465.0</v>
+      </c>
     </row>
     <row r="507" ht="15.75" customHeight="1">
       <c r="A507" s="1">
@@ -16089,16 +16152,37 @@
       <c r="B507" s="4">
         <v>44426.0</v>
       </c>
-      <c r="C507" s="2"/>
-      <c r="D507" s="2"/>
-      <c r="E507" s="2"/>
-      <c r="F507" s="2"/>
-      <c r="G507" s="2"/>
-      <c r="H507" s="2"/>
-      <c r="I507" s="2"/>
-      <c r="J507" s="2"/>
-      <c r="K507" s="2"/>
-      <c r="L507" s="2"/>
+      <c r="C507" s="1">
+        <v>29167.0</v>
+      </c>
+      <c r="D507" s="2">
+        <f t="shared" si="2"/>
+        <v>53</v>
+      </c>
+      <c r="E507" s="1">
+        <v>569.0</v>
+      </c>
+      <c r="F507" s="1">
+        <v>48.0</v>
+      </c>
+      <c r="G507" s="1">
+        <v>47.0</v>
+      </c>
+      <c r="H507" s="1">
+        <v>29.0</v>
+      </c>
+      <c r="I507" s="1">
+        <v>169292.0</v>
+      </c>
+      <c r="J507" s="1">
+        <v>67944.0</v>
+      </c>
+      <c r="K507" s="1">
+        <v>5944.0</v>
+      </c>
+      <c r="L507" s="1">
+        <v>243180.0</v>
+      </c>
     </row>
     <row r="508" ht="15.75" customHeight="1">
       <c r="A508" s="1">
@@ -16108,16 +16192,37 @@
       <c r="B508" s="4">
         <v>44427.0</v>
       </c>
-      <c r="C508" s="2"/>
-      <c r="D508" s="2"/>
-      <c r="E508" s="2"/>
-      <c r="F508" s="2"/>
-      <c r="G508" s="2"/>
-      <c r="H508" s="2"/>
-      <c r="I508" s="2"/>
-      <c r="J508" s="2"/>
-      <c r="K508" s="2"/>
-      <c r="L508" s="2"/>
+      <c r="C508" s="1">
+        <v>29194.0</v>
+      </c>
+      <c r="D508" s="2">
+        <f t="shared" si="2"/>
+        <v>27</v>
+      </c>
+      <c r="E508" s="1">
+        <v>569.0</v>
+      </c>
+      <c r="F508" s="1">
+        <v>43.0</v>
+      </c>
+      <c r="G508" s="1">
+        <v>42.0</v>
+      </c>
+      <c r="H508" s="1">
+        <v>24.0</v>
+      </c>
+      <c r="I508" s="1">
+        <v>171294.0</v>
+      </c>
+      <c r="J508" s="1">
+        <v>69946.0</v>
+      </c>
+      <c r="K508" s="1">
+        <v>5944.0</v>
+      </c>
+      <c r="L508" s="1">
+        <v>247184.0</v>
+      </c>
     </row>
     <row r="509" ht="15.75" customHeight="1">
       <c r="A509" s="1">
@@ -16127,16 +16232,37 @@
       <c r="B509" s="4">
         <v>44428.0</v>
       </c>
-      <c r="C509" s="2"/>
-      <c r="D509" s="2"/>
-      <c r="E509" s="2"/>
-      <c r="F509" s="2"/>
-      <c r="G509" s="2"/>
-      <c r="H509" s="2"/>
-      <c r="I509" s="2"/>
-      <c r="J509" s="2"/>
-      <c r="K509" s="2"/>
-      <c r="L509" s="2"/>
+      <c r="C509" s="1">
+        <v>29225.0</v>
+      </c>
+      <c r="D509" s="2">
+        <f t="shared" si="2"/>
+        <v>31</v>
+      </c>
+      <c r="E509" s="1">
+        <v>570.0</v>
+      </c>
+      <c r="F509" s="1">
+        <v>38.0</v>
+      </c>
+      <c r="G509" s="1">
+        <v>38.0</v>
+      </c>
+      <c r="H509" s="1">
+        <v>22.0</v>
+      </c>
+      <c r="I509" s="1">
+        <v>173042.0</v>
+      </c>
+      <c r="J509" s="1">
+        <v>71889.0</v>
+      </c>
+      <c r="K509" s="1">
+        <v>5944.0</v>
+      </c>
+      <c r="L509" s="1">
+        <v>250875.0</v>
+      </c>
     </row>
     <row r="510" ht="15.75" customHeight="1">
       <c r="A510" s="1">
@@ -16146,16 +16272,37 @@
       <c r="B510" s="4">
         <v>44429.0</v>
       </c>
-      <c r="C510" s="2"/>
-      <c r="D510" s="2"/>
-      <c r="E510" s="2"/>
-      <c r="F510" s="2"/>
-      <c r="G510" s="2"/>
-      <c r="H510" s="2"/>
-      <c r="I510" s="2"/>
-      <c r="J510" s="2"/>
-      <c r="K510" s="2"/>
-      <c r="L510" s="2"/>
+      <c r="C510" s="15">
+        <v>29271.0</v>
+      </c>
+      <c r="D510" s="2">
+        <f t="shared" si="2"/>
+        <v>46</v>
+      </c>
+      <c r="E510" s="15">
+        <v>570.0</v>
+      </c>
+      <c r="F510" s="15">
+        <v>41.0</v>
+      </c>
+      <c r="G510" s="15">
+        <v>41.0</v>
+      </c>
+      <c r="H510" s="15">
+        <v>23.0</v>
+      </c>
+      <c r="I510" s="15">
+        <v>174035.0</v>
+      </c>
+      <c r="J510" s="15">
+        <v>74818.0</v>
+      </c>
+      <c r="K510" s="15">
+        <v>5977.0</v>
+      </c>
+      <c r="L510" s="15">
+        <v>254830.0</v>
+      </c>
     </row>
     <row r="511" ht="15.75" customHeight="1">
       <c r="A511" s="1">
@@ -16831,7 +16978,7 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{12621F90-3527-4EC5-8665-E3613A458E47}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{3048ACAE-E4B1-45E5-83C0-B10EF9140B30}" filter="1" showAutoFilter="1">
       <autoFilter ref="$G$9"/>
       <extLst>
         <ext uri="GoogleSheetsCustomDataVersion1">

</xml_diff>

<commit_message>
Added data on 18 Sep
</commit_message>
<xml_diff>
--- a/Araraquara_covid.xlsx
+++ b/Araraquara_covid.xlsx
@@ -6,11 +6,11 @@
     <sheet state="visible" name="Araraquara covid.csv" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="Z_3D47EBC0_2541_4FA8_B20D_D6C6F15D89F7_.wvu.FilterData">'Araraquara covid.csv'!$G$9</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_88A7EE37_FF51_4D26_B0DB_7723BB5C1D1C_.wvu.FilterData">'Araraquara covid.csv'!$G$9</definedName>
   </definedNames>
   <calcPr/>
   <customWorkbookViews>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{3D47EBC0-2541-4FA8-B20D-D6C6F15D89F7}" name="Filtro 1"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{88A7EE37-FF51-4D26-B0DB-7723BB5C1D1C}" name="Filtro 1"/>
   </customWorkbookViews>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
@@ -115,7 +115,7 @@
   </commentList>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7miAHvS+S3PH0iF91g83oZO50UVhnA=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mjqDJWptaSoO8UbkZGhFqk2raMP/A=="/>
     </ext>
   </extLst>
 </comments>
@@ -630,7 +630,7 @@
         <v>5.0</v>
       </c>
       <c r="D3" s="2">
-        <f t="shared" ref="D3:D537" si="2">(C3-C2)</f>
+        <f t="shared" ref="D3:D538" si="2">(C3-C2)</f>
         <v>2</v>
       </c>
       <c r="E3" s="1">
@@ -17699,38 +17699,38 @@
       <c r="B532" s="5">
         <v>44451.0</v>
       </c>
-      <c r="C532" s="19">
+      <c r="C532" s="1">
         <v>29705.0</v>
       </c>
       <c r="D532" s="2">
         <f t="shared" si="2"/>
         <v>18</v>
       </c>
-      <c r="E532" s="19">
+      <c r="E532" s="1">
         <v>583.0</v>
       </c>
-      <c r="F532" s="19">
+      <c r="F532" s="1">
         <v>13.0</v>
       </c>
-      <c r="G532" s="19">
+      <c r="G532" s="1">
         <v>10.0</v>
       </c>
-      <c r="H532" s="19">
+      <c r="H532" s="1">
         <v>4.0</v>
       </c>
-      <c r="I532" s="19">
+      <c r="I532" s="1">
         <v>186618.0</v>
       </c>
-      <c r="J532" s="19">
+      <c r="J532" s="1">
         <v>109075.0</v>
       </c>
-      <c r="K532" s="19">
-        <v>0.0</v>
-      </c>
-      <c r="L532" s="19">
+      <c r="K532" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="L532" s="1">
         <v>47.0</v>
       </c>
-      <c r="M532" s="19">
+      <c r="M532" s="1">
         <v>295740.0</v>
       </c>
     </row>
@@ -17742,38 +17742,38 @@
       <c r="B533" s="5">
         <v>44452.0</v>
       </c>
-      <c r="C533" s="19">
+      <c r="C533" s="1">
         <v>29712.0</v>
       </c>
       <c r="D533" s="2">
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
-      <c r="E533" s="19">
+      <c r="E533" s="1">
         <v>583.0</v>
       </c>
-      <c r="F533" s="19">
+      <c r="F533" s="1">
         <v>17.0</v>
       </c>
-      <c r="G533" s="19">
+      <c r="G533" s="1">
         <v>14.0</v>
       </c>
-      <c r="H533" s="19">
+      <c r="H533" s="1">
         <v>3.0</v>
       </c>
-      <c r="I533" s="19">
+      <c r="I533" s="1">
         <v>186618.0</v>
       </c>
-      <c r="J533" s="19">
+      <c r="J533" s="1">
         <v>109075.0</v>
       </c>
-      <c r="K533" s="19">
-        <v>0.0</v>
-      </c>
-      <c r="L533" s="19">
+      <c r="K533" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="L533" s="1">
         <v>47.0</v>
       </c>
-      <c r="M533" s="19">
+      <c r="M533" s="1">
         <v>295740.0</v>
       </c>
     </row>
@@ -17785,38 +17785,38 @@
       <c r="B534" s="5">
         <v>44453.0</v>
       </c>
-      <c r="C534" s="19">
+      <c r="C534" s="1">
         <v>29762.0</v>
       </c>
       <c r="D534" s="2">
         <f t="shared" si="2"/>
         <v>50</v>
       </c>
-      <c r="E534" s="19">
+      <c r="E534" s="1">
         <v>583.0</v>
       </c>
-      <c r="F534" s="19">
+      <c r="F534" s="1">
         <v>17.0</v>
       </c>
-      <c r="G534" s="19">
+      <c r="G534" s="1">
         <v>15.0</v>
       </c>
-      <c r="H534" s="19">
+      <c r="H534" s="1">
         <v>4.0</v>
       </c>
-      <c r="I534" s="19">
+      <c r="I534" s="1">
         <v>188440.0</v>
       </c>
-      <c r="J534" s="19">
+      <c r="J534" s="1">
         <v>113289.0</v>
       </c>
-      <c r="K534" s="19">
-        <v>0.0</v>
-      </c>
-      <c r="L534" s="19">
+      <c r="K534" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="L534" s="1">
         <v>78.0</v>
       </c>
-      <c r="M534" s="19">
+      <c r="M534" s="1">
         <v>301807.0</v>
       </c>
     </row>
@@ -17828,38 +17828,38 @@
       <c r="B535" s="5">
         <v>44454.0</v>
       </c>
-      <c r="C535" s="19">
+      <c r="C535" s="1">
         <v>29792.0</v>
       </c>
       <c r="D535" s="2">
         <f t="shared" si="2"/>
         <v>30</v>
       </c>
-      <c r="E535" s="19">
+      <c r="E535" s="1">
         <v>583.0</v>
       </c>
-      <c r="F535" s="19">
+      <c r="F535" s="1">
         <v>18.0</v>
       </c>
-      <c r="G535" s="19">
+      <c r="G535" s="1">
         <v>17.0</v>
       </c>
-      <c r="H535" s="19">
+      <c r="H535" s="1">
         <v>4.0</v>
       </c>
-      <c r="I535" s="19">
+      <c r="I535" s="1">
         <v>189159.0</v>
       </c>
-      <c r="J535" s="19">
+      <c r="J535" s="1">
         <v>116747.0</v>
       </c>
-      <c r="K535" s="19">
-        <v>0.0</v>
-      </c>
-      <c r="L535" s="19">
+      <c r="K535" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="L535" s="1">
         <v>123.0</v>
       </c>
-      <c r="M535" s="19">
+      <c r="M535" s="1">
         <v>306029.0</v>
       </c>
     </row>
@@ -17871,38 +17871,38 @@
       <c r="B536" s="5">
         <v>44455.0</v>
       </c>
-      <c r="C536" s="19">
+      <c r="C536" s="1">
         <v>29836.0</v>
       </c>
       <c r="D536" s="2">
         <f t="shared" si="2"/>
         <v>44</v>
       </c>
-      <c r="E536" s="19">
+      <c r="E536" s="1">
         <v>583.0</v>
       </c>
-      <c r="F536" s="19">
+      <c r="F536" s="1">
         <v>20.0</v>
       </c>
-      <c r="G536" s="19">
+      <c r="G536" s="1">
         <v>18.0</v>
       </c>
-      <c r="H536" s="19">
+      <c r="H536" s="1">
         <v>4.0</v>
       </c>
-      <c r="I536" s="19">
+      <c r="I536" s="1">
         <v>190380.0</v>
       </c>
-      <c r="J536" s="19">
+      <c r="J536" s="1">
         <v>119097.0</v>
       </c>
-      <c r="K536" s="19">
-        <v>0.0</v>
-      </c>
-      <c r="L536" s="19">
+      <c r="K536" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="L536" s="1">
         <v>241.0</v>
       </c>
-      <c r="M536" s="19">
+      <c r="M536" s="1">
         <v>309718.0</v>
       </c>
     </row>
@@ -17914,38 +17914,38 @@
       <c r="B537" s="5">
         <v>44456.0</v>
       </c>
-      <c r="C537" s="19">
+      <c r="C537" s="1">
         <v>29880.0</v>
       </c>
       <c r="D537" s="2">
         <f t="shared" si="2"/>
         <v>44</v>
       </c>
-      <c r="E537" s="19">
+      <c r="E537" s="1">
         <v>583.0</v>
       </c>
-      <c r="F537" s="19">
+      <c r="F537" s="1">
         <v>21.0</v>
       </c>
-      <c r="G537" s="19">
+      <c r="G537" s="1">
         <v>17.0</v>
       </c>
-      <c r="H537" s="19">
+      <c r="H537" s="1">
         <v>2.0</v>
       </c>
-      <c r="I537" s="19">
+      <c r="I537" s="1">
         <v>191214.0</v>
       </c>
-      <c r="J537" s="19">
+      <c r="J537" s="1">
         <v>121655.0</v>
       </c>
-      <c r="K537" s="19">
-        <v>0.0</v>
-      </c>
-      <c r="L537" s="19">
+      <c r="K537" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="L537" s="1">
         <v>369.0</v>
       </c>
-      <c r="M537" s="19">
+      <c r="M537" s="1">
         <v>313238.0</v>
       </c>
     </row>
@@ -17957,17 +17957,40 @@
       <c r="B538" s="5">
         <v>44457.0</v>
       </c>
-      <c r="C538" s="2"/>
-      <c r="D538" s="2"/>
-      <c r="E538" s="2"/>
-      <c r="F538" s="2"/>
-      <c r="G538" s="2"/>
-      <c r="H538" s="2"/>
-      <c r="I538" s="2"/>
-      <c r="J538" s="2"/>
-      <c r="K538" s="2"/>
-      <c r="L538" s="2"/>
-      <c r="M538" s="2"/>
+      <c r="C538" s="19">
+        <v>29917.0</v>
+      </c>
+      <c r="D538" s="2">
+        <f t="shared" si="2"/>
+        <v>37</v>
+      </c>
+      <c r="E538" s="19">
+        <v>583.0</v>
+      </c>
+      <c r="F538" s="19">
+        <v>20.0</v>
+      </c>
+      <c r="G538" s="19">
+        <v>18.0</v>
+      </c>
+      <c r="H538" s="19">
+        <v>4.0</v>
+      </c>
+      <c r="I538" s="19">
+        <v>192207.0</v>
+      </c>
+      <c r="J538" s="19">
+        <v>124347.0</v>
+      </c>
+      <c r="K538" s="19">
+        <v>0.0</v>
+      </c>
+      <c r="L538" s="19">
+        <v>524.0</v>
+      </c>
+      <c r="M538" s="19">
+        <v>317078.0</v>
+      </c>
     </row>
     <row r="539" ht="15.75" customHeight="1">
       <c r="A539" s="1">
@@ -18661,7 +18684,7 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{3D47EBC0-2541-4FA8-B20D-D6C6F15D89F7}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{88A7EE37-FF51-4D26-B0DB-7723BB5C1D1C}" filter="1" showAutoFilter="1">
       <autoFilter ref="$G$9"/>
       <extLst>
         <ext uri="GoogleSheetsCustomDataVersion1">

</xml_diff>

<commit_message>
Added data on 2 Oct
</commit_message>
<xml_diff>
--- a/Araraquara_covid.xlsx
+++ b/Araraquara_covid.xlsx
@@ -6,15 +6,15 @@
     <sheet state="visible" name="Araraquara covid.csv" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="Z_88A7EE37_FF51_4D26_B0DB_7723BB5C1D1C_.wvu.FilterData">'Araraquara covid.csv'!$G$9</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_B5C5D958_6324_40D8_B4E1_76BBA7389C94_.wvu.FilterData">'Araraquara covid.csv'!$G$9</definedName>
   </definedNames>
   <calcPr/>
   <customWorkbookViews>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{88A7EE37-FF51-4D26-B0DB-7723BB5C1D1C}" name="Filtro 1"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{B5C5D958-6324-40D8-B4E1-76BBA7389C94}" name="Filtro 1"/>
   </customWorkbookViews>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mi0rmjeiBQm4x3+fU+J16YuQuflDQ=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mj/E0YO6oMf7E2klD9t4mGgJXT68w=="/>
     </ext>
   </extLst>
 </workbook>
@@ -26,6 +26,14 @@
     <author/>
   </authors>
   <commentList>
+    <comment authorId="0" ref="J547">
+      <text>
+        <t xml:space="preserve">======
+ID#AAAAQkWK1fQ
+Daniel Nogueira Hammer    (2021-10-02 23:04:12)
+No boletim da prefeitura está 139734. Esse número é menor do que o do dia anterior. Ao olhar o texto, diz que foram registrados 133731+6063 = 139.794</t>
+      </text>
+    </comment>
     <comment authorId="0" ref="J1">
       <text>
         <t xml:space="preserve">======
@@ -115,7 +123,7 @@
   </commentList>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mjqDJWptaSoO8UbkZGhFqk2raMP/A=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mhsCv6ErEnzZl9lc9UDQB1vUrdLhw=="/>
     </ext>
   </extLst>
 </comments>
@@ -252,7 +260,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -311,6 +319,12 @@
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="6" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -620,7 +634,7 @@
     </row>
     <row r="3">
       <c r="A3" s="1">
-        <f t="shared" ref="A3:A550" si="1">A2+1</f>
+        <f t="shared" ref="A3:A581" si="1">A2+1</f>
         <v>1</v>
       </c>
       <c r="B3" s="5">
@@ -630,7 +644,7 @@
         <v>5.0</v>
       </c>
       <c r="D3" s="2">
-        <f t="shared" ref="D3:D538" si="2">(C3-C2)</f>
+        <f t="shared" ref="D3:D552" si="2">(C3-C2)</f>
         <v>2</v>
       </c>
       <c r="E3" s="1">
@@ -17957,38 +17971,38 @@
       <c r="B538" s="5">
         <v>44457.0</v>
       </c>
-      <c r="C538" s="19">
+      <c r="C538" s="1">
         <v>29917.0</v>
       </c>
       <c r="D538" s="2">
         <f t="shared" si="2"/>
         <v>37</v>
       </c>
-      <c r="E538" s="19">
+      <c r="E538" s="1">
         <v>583.0</v>
       </c>
-      <c r="F538" s="19">
+      <c r="F538" s="1">
         <v>20.0</v>
       </c>
-      <c r="G538" s="19">
+      <c r="G538" s="1">
         <v>18.0</v>
       </c>
-      <c r="H538" s="19">
+      <c r="H538" s="1">
         <v>4.0</v>
       </c>
-      <c r="I538" s="19">
+      <c r="I538" s="1">
         <v>192207.0</v>
       </c>
-      <c r="J538" s="19">
+      <c r="J538" s="1">
         <v>124347.0</v>
       </c>
-      <c r="K538" s="19">
-        <v>0.0</v>
-      </c>
-      <c r="L538" s="19">
+      <c r="K538" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="L538" s="1">
         <v>524.0</v>
       </c>
-      <c r="M538" s="19">
+      <c r="M538" s="1">
         <v>317078.0</v>
       </c>
     </row>
@@ -18000,17 +18014,40 @@
       <c r="B539" s="5">
         <v>44458.0</v>
       </c>
-      <c r="C539" s="2"/>
-      <c r="D539" s="2"/>
-      <c r="E539" s="2"/>
-      <c r="F539" s="2"/>
-      <c r="G539" s="2"/>
-      <c r="H539" s="2"/>
-      <c r="I539" s="2"/>
-      <c r="J539" s="2"/>
-      <c r="K539" s="2"/>
-      <c r="L539" s="2"/>
-      <c r="M539" s="2"/>
+      <c r="C539" s="19">
+        <v>29951.0</v>
+      </c>
+      <c r="D539" s="2">
+        <f t="shared" si="2"/>
+        <v>34</v>
+      </c>
+      <c r="E539" s="19">
+        <v>584.0</v>
+      </c>
+      <c r="F539" s="19">
+        <v>18.0</v>
+      </c>
+      <c r="G539" s="19">
+        <v>17.0</v>
+      </c>
+      <c r="H539" s="19">
+        <v>5.0</v>
+      </c>
+      <c r="I539" s="19">
+        <v>192410.0</v>
+      </c>
+      <c r="J539" s="19">
+        <v>125022.0</v>
+      </c>
+      <c r="K539" s="19">
+        <v>0.0</v>
+      </c>
+      <c r="L539" s="19">
+        <v>890.0</v>
+      </c>
+      <c r="M539" s="19">
+        <v>318322.0</v>
+      </c>
     </row>
     <row r="540" ht="15.75" customHeight="1">
       <c r="A540" s="1">
@@ -18020,17 +18057,40 @@
       <c r="B540" s="5">
         <v>44459.0</v>
       </c>
-      <c r="C540" s="2"/>
-      <c r="D540" s="2"/>
-      <c r="E540" s="2"/>
-      <c r="F540" s="2"/>
-      <c r="G540" s="2"/>
-      <c r="H540" s="2"/>
-      <c r="I540" s="2"/>
-      <c r="J540" s="2"/>
-      <c r="K540" s="2"/>
-      <c r="L540" s="2"/>
-      <c r="M540" s="2"/>
+      <c r="C540" s="19">
+        <v>29956.0</v>
+      </c>
+      <c r="D540" s="2">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="E540" s="19">
+        <v>584.0</v>
+      </c>
+      <c r="F540" s="19">
+        <v>18.0</v>
+      </c>
+      <c r="G540" s="19">
+        <v>17.0</v>
+      </c>
+      <c r="H540" s="19">
+        <v>5.0</v>
+      </c>
+      <c r="I540" s="19">
+        <v>192472.0</v>
+      </c>
+      <c r="J540" s="19">
+        <v>125409.0</v>
+      </c>
+      <c r="K540" s="19">
+        <v>0.0</v>
+      </c>
+      <c r="L540" s="19">
+        <v>900.0</v>
+      </c>
+      <c r="M540" s="19">
+        <v>318781.0</v>
+      </c>
     </row>
     <row r="541" ht="15.75" customHeight="1">
       <c r="A541" s="1">
@@ -18040,17 +18100,40 @@
       <c r="B541" s="5">
         <v>44460.0</v>
       </c>
-      <c r="C541" s="2"/>
-      <c r="D541" s="2"/>
-      <c r="E541" s="2"/>
-      <c r="F541" s="2"/>
-      <c r="G541" s="2"/>
-      <c r="H541" s="2"/>
-      <c r="I541" s="2"/>
-      <c r="J541" s="2"/>
-      <c r="K541" s="2"/>
-      <c r="L541" s="2"/>
-      <c r="M541" s="2"/>
+      <c r="C541" s="19">
+        <v>30014.0</v>
+      </c>
+      <c r="D541" s="2">
+        <f t="shared" si="2"/>
+        <v>58</v>
+      </c>
+      <c r="E541" s="19">
+        <v>584.0</v>
+      </c>
+      <c r="F541" s="19">
+        <v>17.0</v>
+      </c>
+      <c r="G541" s="19">
+        <v>16.0</v>
+      </c>
+      <c r="H541" s="19">
+        <v>5.0</v>
+      </c>
+      <c r="I541" s="19">
+        <v>192943.0</v>
+      </c>
+      <c r="J541" s="19">
+        <v>127253.0</v>
+      </c>
+      <c r="K541" s="19">
+        <v>0.0</v>
+      </c>
+      <c r="L541" s="19">
+        <v>979.0</v>
+      </c>
+      <c r="M541" s="19">
+        <v>321175.0</v>
+      </c>
     </row>
     <row r="542" ht="15.75" customHeight="1">
       <c r="A542" s="1">
@@ -18060,17 +18143,40 @@
       <c r="B542" s="5">
         <v>44461.0</v>
       </c>
-      <c r="C542" s="2"/>
-      <c r="D542" s="2"/>
-      <c r="E542" s="2"/>
-      <c r="F542" s="2"/>
-      <c r="G542" s="2"/>
-      <c r="H542" s="2"/>
-      <c r="I542" s="2"/>
-      <c r="J542" s="2"/>
-      <c r="K542" s="2"/>
-      <c r="L542" s="2"/>
-      <c r="M542" s="2"/>
+      <c r="C542" s="19">
+        <v>30053.0</v>
+      </c>
+      <c r="D542" s="2">
+        <f t="shared" si="2"/>
+        <v>39</v>
+      </c>
+      <c r="E542" s="19">
+        <v>584.0</v>
+      </c>
+      <c r="F542" s="19">
+        <v>17.0</v>
+      </c>
+      <c r="G542" s="19">
+        <v>16.0</v>
+      </c>
+      <c r="H542" s="19">
+        <v>4.0</v>
+      </c>
+      <c r="I542" s="19">
+        <v>193302.0</v>
+      </c>
+      <c r="J542" s="19">
+        <v>129966.0</v>
+      </c>
+      <c r="K542" s="19">
+        <v>0.0</v>
+      </c>
+      <c r="L542" s="19">
+        <v>1129.0</v>
+      </c>
+      <c r="M542" s="19">
+        <v>324397.0</v>
+      </c>
     </row>
     <row r="543" ht="15.75" customHeight="1">
       <c r="A543" s="1">
@@ -18080,17 +18186,40 @@
       <c r="B543" s="5">
         <v>44462.0</v>
       </c>
-      <c r="C543" s="2"/>
-      <c r="D543" s="2"/>
-      <c r="E543" s="2"/>
-      <c r="F543" s="2"/>
-      <c r="G543" s="2"/>
-      <c r="H543" s="2"/>
-      <c r="I543" s="2"/>
-      <c r="J543" s="2"/>
-      <c r="K543" s="2"/>
-      <c r="L543" s="2"/>
-      <c r="M543" s="2"/>
+      <c r="C543" s="19">
+        <v>30115.0</v>
+      </c>
+      <c r="D543" s="2">
+        <f t="shared" si="2"/>
+        <v>62</v>
+      </c>
+      <c r="E543" s="19">
+        <v>584.0</v>
+      </c>
+      <c r="F543" s="19">
+        <v>14.0</v>
+      </c>
+      <c r="G543" s="19">
+        <v>14.0</v>
+      </c>
+      <c r="H543" s="19">
+        <v>4.0</v>
+      </c>
+      <c r="I543" s="19">
+        <v>193558.0</v>
+      </c>
+      <c r="J543" s="19">
+        <v>132558.0</v>
+      </c>
+      <c r="K543" s="19">
+        <v>0.0</v>
+      </c>
+      <c r="L543" s="19">
+        <v>1408.0</v>
+      </c>
+      <c r="M543" s="19">
+        <v>327524.0</v>
+      </c>
     </row>
     <row r="544" ht="15.75" customHeight="1">
       <c r="A544" s="1">
@@ -18100,17 +18229,40 @@
       <c r="B544" s="5">
         <v>44463.0</v>
       </c>
-      <c r="C544" s="2"/>
-      <c r="D544" s="2"/>
-      <c r="E544" s="2"/>
-      <c r="F544" s="2"/>
-      <c r="G544" s="2"/>
-      <c r="H544" s="2"/>
-      <c r="I544" s="2"/>
-      <c r="J544" s="2"/>
-      <c r="K544" s="2"/>
-      <c r="L544" s="2"/>
-      <c r="M544" s="2"/>
+      <c r="C544" s="19">
+        <v>30144.0</v>
+      </c>
+      <c r="D544" s="2">
+        <f t="shared" si="2"/>
+        <v>29</v>
+      </c>
+      <c r="E544" s="19">
+        <v>584.0</v>
+      </c>
+      <c r="F544" s="19">
+        <v>18.0</v>
+      </c>
+      <c r="G544" s="19">
+        <v>16.0</v>
+      </c>
+      <c r="H544" s="19">
+        <v>8.0</v>
+      </c>
+      <c r="I544" s="19">
+        <v>193860.0</v>
+      </c>
+      <c r="J544" s="19">
+        <v>135291.0</v>
+      </c>
+      <c r="K544" s="19">
+        <v>0.0</v>
+      </c>
+      <c r="L544" s="19">
+        <v>1512.0</v>
+      </c>
+      <c r="M544" s="19">
+        <v>330663.0</v>
+      </c>
     </row>
     <row r="545" ht="15.75" customHeight="1">
       <c r="A545" s="1">
@@ -18120,17 +18272,40 @@
       <c r="B545" s="5">
         <v>44464.0</v>
       </c>
-      <c r="C545" s="2"/>
-      <c r="D545" s="2"/>
-      <c r="E545" s="2"/>
-      <c r="F545" s="2"/>
-      <c r="G545" s="2"/>
-      <c r="H545" s="2"/>
-      <c r="I545" s="2"/>
-      <c r="J545" s="2"/>
-      <c r="K545" s="2"/>
-      <c r="L545" s="2"/>
-      <c r="M545" s="2"/>
+      <c r="C545" s="19">
+        <v>30186.0</v>
+      </c>
+      <c r="D545" s="2">
+        <f t="shared" si="2"/>
+        <v>42</v>
+      </c>
+      <c r="E545" s="19">
+        <v>584.0</v>
+      </c>
+      <c r="F545" s="19">
+        <v>15.0</v>
+      </c>
+      <c r="G545" s="19">
+        <v>14.0</v>
+      </c>
+      <c r="H545" s="19">
+        <v>7.0</v>
+      </c>
+      <c r="I545" s="19">
+        <v>194056.0</v>
+      </c>
+      <c r="J545" s="19">
+        <v>138108.0</v>
+      </c>
+      <c r="K545" s="19">
+        <v>0.0</v>
+      </c>
+      <c r="L545" s="19">
+        <v>1681.0</v>
+      </c>
+      <c r="M545" s="19">
+        <v>333845.0</v>
+      </c>
     </row>
     <row r="546" ht="15.75" customHeight="1">
       <c r="A546" s="1">
@@ -18140,17 +18315,40 @@
       <c r="B546" s="5">
         <v>44465.0</v>
       </c>
-      <c r="C546" s="2"/>
-      <c r="D546" s="2"/>
-      <c r="E546" s="2"/>
-      <c r="F546" s="2"/>
-      <c r="G546" s="2"/>
-      <c r="H546" s="2"/>
-      <c r="I546" s="2"/>
-      <c r="J546" s="2"/>
-      <c r="K546" s="2"/>
-      <c r="L546" s="2"/>
-      <c r="M546" s="2"/>
+      <c r="C546" s="19">
+        <v>30224.0</v>
+      </c>
+      <c r="D546" s="2">
+        <f t="shared" si="2"/>
+        <v>38</v>
+      </c>
+      <c r="E546" s="19">
+        <v>585.0</v>
+      </c>
+      <c r="F546" s="19">
+        <v>17.0</v>
+      </c>
+      <c r="G546" s="19">
+        <v>14.0</v>
+      </c>
+      <c r="H546" s="19">
+        <v>7.0</v>
+      </c>
+      <c r="I546" s="19">
+        <v>194187.0</v>
+      </c>
+      <c r="J546" s="19">
+        <v>139779.0</v>
+      </c>
+      <c r="K546" s="19">
+        <v>0.0</v>
+      </c>
+      <c r="L546" s="19">
+        <v>1770.0</v>
+      </c>
+      <c r="M546" s="19">
+        <v>335736.0</v>
+      </c>
     </row>
     <row r="547" ht="15.75" customHeight="1">
       <c r="A547" s="1">
@@ -18160,17 +18358,40 @@
       <c r="B547" s="5">
         <v>44466.0</v>
       </c>
-      <c r="C547" s="2"/>
-      <c r="D547" s="2"/>
-      <c r="E547" s="2"/>
-      <c r="F547" s="2"/>
-      <c r="G547" s="2"/>
-      <c r="H547" s="2"/>
-      <c r="I547" s="2"/>
-      <c r="J547" s="2"/>
-      <c r="K547" s="2"/>
-      <c r="L547" s="2"/>
-      <c r="M547" s="2"/>
+      <c r="C547" s="19">
+        <v>30237.0</v>
+      </c>
+      <c r="D547" s="2">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="E547" s="19">
+        <v>586.0</v>
+      </c>
+      <c r="F547" s="19">
+        <v>19.0</v>
+      </c>
+      <c r="G547" s="19">
+        <v>15.0</v>
+      </c>
+      <c r="H547" s="19">
+        <v>7.0</v>
+      </c>
+      <c r="I547" s="19">
+        <v>194191.0</v>
+      </c>
+      <c r="J547" s="20">
+        <v>139794.0</v>
+      </c>
+      <c r="K547" s="19">
+        <v>0.0</v>
+      </c>
+      <c r="L547" s="16">
+        <v>1770.0</v>
+      </c>
+      <c r="M547" s="19">
+        <v>335755.0</v>
+      </c>
     </row>
     <row r="548" ht="15.75" customHeight="1">
       <c r="A548" s="1">
@@ -18180,17 +18401,40 @@
       <c r="B548" s="5">
         <v>44467.0</v>
       </c>
-      <c r="C548" s="2"/>
-      <c r="D548" s="2"/>
-      <c r="E548" s="2"/>
-      <c r="F548" s="2"/>
-      <c r="G548" s="2"/>
-      <c r="H548" s="2"/>
-      <c r="I548" s="2"/>
-      <c r="J548" s="2"/>
-      <c r="K548" s="2"/>
-      <c r="L548" s="2"/>
-      <c r="M548" s="2"/>
+      <c r="C548" s="19">
+        <v>30270.0</v>
+      </c>
+      <c r="D548" s="2">
+        <f t="shared" si="2"/>
+        <v>33</v>
+      </c>
+      <c r="E548" s="19">
+        <v>586.0</v>
+      </c>
+      <c r="F548" s="19">
+        <v>19.0</v>
+      </c>
+      <c r="G548" s="19">
+        <v>16.0</v>
+      </c>
+      <c r="H548" s="19">
+        <v>7.0</v>
+      </c>
+      <c r="I548" s="19">
+        <v>194366.0</v>
+      </c>
+      <c r="J548" s="19">
+        <v>141731.0</v>
+      </c>
+      <c r="K548" s="19">
+        <v>0.0</v>
+      </c>
+      <c r="L548" s="19">
+        <v>1796.0</v>
+      </c>
+      <c r="M548" s="19">
+        <v>337893.0</v>
+      </c>
     </row>
     <row r="549" ht="15.75" customHeight="1">
       <c r="A549" s="1">
@@ -18200,17 +18444,40 @@
       <c r="B549" s="5">
         <v>44468.0</v>
       </c>
-      <c r="C549" s="2"/>
-      <c r="D549" s="2"/>
-      <c r="E549" s="2"/>
-      <c r="F549" s="2"/>
-      <c r="G549" s="2"/>
-      <c r="H549" s="2"/>
-      <c r="I549" s="2"/>
-      <c r="J549" s="2"/>
-      <c r="K549" s="2"/>
-      <c r="L549" s="2"/>
-      <c r="M549" s="2"/>
+      <c r="C549" s="19">
+        <v>30298.0</v>
+      </c>
+      <c r="D549" s="2">
+        <f t="shared" si="2"/>
+        <v>28</v>
+      </c>
+      <c r="E549" s="19">
+        <v>586.0</v>
+      </c>
+      <c r="F549" s="19">
+        <v>19.0</v>
+      </c>
+      <c r="G549" s="19">
+        <v>17.0</v>
+      </c>
+      <c r="H549" s="19">
+        <v>6.0</v>
+      </c>
+      <c r="I549" s="19">
+        <v>194690.0</v>
+      </c>
+      <c r="J549" s="19">
+        <v>145463.0</v>
+      </c>
+      <c r="K549" s="19">
+        <v>0.0</v>
+      </c>
+      <c r="L549" s="19">
+        <v>1939.0</v>
+      </c>
+      <c r="M549" s="19">
+        <v>342092.0</v>
+      </c>
     </row>
     <row r="550" ht="15.75" customHeight="1">
       <c r="A550" s="1">
@@ -18220,50 +18487,710 @@
       <c r="B550" s="5">
         <v>44469.0</v>
       </c>
-      <c r="C550" s="2"/>
-      <c r="D550" s="2"/>
-      <c r="E550" s="2"/>
-      <c r="F550" s="2"/>
-      <c r="G550" s="2"/>
-      <c r="H550" s="2"/>
-      <c r="I550" s="2"/>
-      <c r="J550" s="2"/>
-      <c r="K550" s="2"/>
-      <c r="L550" s="2"/>
-      <c r="M550" s="2"/>
-    </row>
-    <row r="551" ht="15.75" customHeight="1"/>
-    <row r="552" ht="15.75" customHeight="1"/>
-    <row r="553" ht="15.75" customHeight="1"/>
-    <row r="554" ht="15.75" customHeight="1"/>
-    <row r="555" ht="15.75" customHeight="1"/>
-    <row r="556" ht="15.75" customHeight="1"/>
-    <row r="557" ht="15.75" customHeight="1"/>
-    <row r="558" ht="15.75" customHeight="1"/>
-    <row r="559" ht="15.75" customHeight="1"/>
-    <row r="560" ht="15.75" customHeight="1"/>
-    <row r="561" ht="15.75" customHeight="1"/>
-    <row r="562" ht="15.75" customHeight="1"/>
-    <row r="563" ht="15.75" customHeight="1"/>
-    <row r="564" ht="15.75" customHeight="1"/>
-    <row r="565" ht="15.75" customHeight="1"/>
-    <row r="566" ht="15.75" customHeight="1"/>
-    <row r="567" ht="15.75" customHeight="1"/>
-    <row r="568" ht="15.75" customHeight="1"/>
-    <row r="569" ht="15.75" customHeight="1"/>
-    <row r="570" ht="15.75" customHeight="1"/>
-    <row r="571" ht="15.75" customHeight="1"/>
-    <row r="572" ht="15.75" customHeight="1"/>
-    <row r="573" ht="15.75" customHeight="1"/>
-    <row r="574" ht="15.75" customHeight="1"/>
-    <row r="575" ht="15.75" customHeight="1"/>
-    <row r="576" ht="15.75" customHeight="1"/>
-    <row r="577" ht="15.75" customHeight="1"/>
-    <row r="578" ht="15.75" customHeight="1"/>
-    <row r="579" ht="15.75" customHeight="1"/>
-    <row r="580" ht="15.75" customHeight="1"/>
-    <row r="581" ht="15.75" customHeight="1"/>
-    <row r="582" ht="15.75" customHeight="1"/>
+      <c r="C550" s="19">
+        <v>30328.0</v>
+      </c>
+      <c r="D550" s="2">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="E550" s="19">
+        <v>586.0</v>
+      </c>
+      <c r="F550" s="19">
+        <v>18.0</v>
+      </c>
+      <c r="G550" s="19">
+        <v>15.0</v>
+      </c>
+      <c r="H550" s="19">
+        <v>8.0</v>
+      </c>
+      <c r="I550" s="19">
+        <v>195016.0</v>
+      </c>
+      <c r="J550" s="19">
+        <v>148922.0</v>
+      </c>
+      <c r="K550" s="19">
+        <v>0.0</v>
+      </c>
+      <c r="L550" s="19">
+        <v>2136.0</v>
+      </c>
+      <c r="M550" s="19">
+        <v>346074.0</v>
+      </c>
+    </row>
+    <row r="551" ht="15.75" customHeight="1">
+      <c r="A551" s="1">
+        <f t="shared" si="1"/>
+        <v>549</v>
+      </c>
+      <c r="B551" s="21">
+        <v>44470.0</v>
+      </c>
+      <c r="C551" s="19">
+        <v>30347.0</v>
+      </c>
+      <c r="D551" s="2">
+        <f t="shared" si="2"/>
+        <v>19</v>
+      </c>
+      <c r="E551" s="19">
+        <v>586.0</v>
+      </c>
+      <c r="F551" s="19">
+        <v>20.0</v>
+      </c>
+      <c r="G551" s="19">
+        <v>18.0</v>
+      </c>
+      <c r="H551" s="19">
+        <v>8.0</v>
+      </c>
+      <c r="I551" s="19">
+        <v>195272.0</v>
+      </c>
+      <c r="J551" s="19">
+        <v>150761.0</v>
+      </c>
+      <c r="K551" s="19">
+        <v>0.0</v>
+      </c>
+      <c r="L551" s="19">
+        <v>2290.0</v>
+      </c>
+      <c r="M551" s="19">
+        <v>348323.0</v>
+      </c>
+    </row>
+    <row r="552" ht="15.75" customHeight="1">
+      <c r="A552" s="1">
+        <f t="shared" si="1"/>
+        <v>550</v>
+      </c>
+      <c r="B552" s="21">
+        <v>44471.0</v>
+      </c>
+      <c r="C552" s="19">
+        <v>30366.0</v>
+      </c>
+      <c r="D552" s="2">
+        <f t="shared" si="2"/>
+        <v>19</v>
+      </c>
+      <c r="E552" s="19">
+        <v>586.0</v>
+      </c>
+      <c r="F552" s="19">
+        <v>18.0</v>
+      </c>
+      <c r="G552" s="19">
+        <v>18.0</v>
+      </c>
+      <c r="H552" s="19">
+        <v>9.0</v>
+      </c>
+      <c r="I552" s="19">
+        <v>195552.0</v>
+      </c>
+      <c r="J552" s="19">
+        <v>152424.0</v>
+      </c>
+      <c r="K552" s="19">
+        <v>0.0</v>
+      </c>
+      <c r="L552" s="19">
+        <v>2375.0</v>
+      </c>
+      <c r="M552" s="19">
+        <v>350351.0</v>
+      </c>
+    </row>
+    <row r="553" ht="15.75" customHeight="1">
+      <c r="A553" s="1">
+        <f t="shared" si="1"/>
+        <v>551</v>
+      </c>
+      <c r="B553" s="21">
+        <v>44472.0</v>
+      </c>
+      <c r="C553" s="2"/>
+      <c r="D553" s="2"/>
+      <c r="E553" s="2"/>
+      <c r="F553" s="2"/>
+      <c r="G553" s="2"/>
+      <c r="H553" s="2"/>
+      <c r="I553" s="2"/>
+      <c r="J553" s="2"/>
+      <c r="K553" s="2"/>
+      <c r="L553" s="2"/>
+      <c r="M553" s="2"/>
+    </row>
+    <row r="554" ht="15.75" customHeight="1">
+      <c r="A554" s="1">
+        <f t="shared" si="1"/>
+        <v>552</v>
+      </c>
+      <c r="B554" s="21">
+        <v>44473.0</v>
+      </c>
+      <c r="C554" s="2"/>
+      <c r="D554" s="2"/>
+      <c r="E554" s="2"/>
+      <c r="F554" s="2"/>
+      <c r="G554" s="2"/>
+      <c r="H554" s="2"/>
+      <c r="I554" s="2"/>
+      <c r="J554" s="2"/>
+      <c r="K554" s="2"/>
+      <c r="L554" s="2"/>
+      <c r="M554" s="2"/>
+    </row>
+    <row r="555" ht="15.75" customHeight="1">
+      <c r="A555" s="1">
+        <f t="shared" si="1"/>
+        <v>553</v>
+      </c>
+      <c r="B555" s="21">
+        <v>44474.0</v>
+      </c>
+      <c r="C555" s="2"/>
+      <c r="D555" s="2"/>
+      <c r="E555" s="2"/>
+      <c r="F555" s="2"/>
+      <c r="G555" s="2"/>
+      <c r="H555" s="2"/>
+      <c r="I555" s="2"/>
+      <c r="J555" s="2"/>
+      <c r="K555" s="2"/>
+      <c r="L555" s="2"/>
+      <c r="M555" s="2"/>
+    </row>
+    <row r="556" ht="15.75" customHeight="1">
+      <c r="A556" s="1">
+        <f t="shared" si="1"/>
+        <v>554</v>
+      </c>
+      <c r="B556" s="21">
+        <v>44475.0</v>
+      </c>
+      <c r="C556" s="2"/>
+      <c r="D556" s="2"/>
+      <c r="E556" s="2"/>
+      <c r="F556" s="2"/>
+      <c r="G556" s="2"/>
+      <c r="H556" s="2"/>
+      <c r="I556" s="2"/>
+      <c r="J556" s="2"/>
+      <c r="K556" s="2"/>
+      <c r="L556" s="2"/>
+      <c r="M556" s="2"/>
+    </row>
+    <row r="557" ht="15.75" customHeight="1">
+      <c r="A557" s="1">
+        <f t="shared" si="1"/>
+        <v>555</v>
+      </c>
+      <c r="B557" s="21">
+        <v>44476.0</v>
+      </c>
+      <c r="C557" s="2"/>
+      <c r="D557" s="2"/>
+      <c r="E557" s="2"/>
+      <c r="F557" s="2"/>
+      <c r="G557" s="2"/>
+      <c r="H557" s="2"/>
+      <c r="I557" s="2"/>
+      <c r="J557" s="2"/>
+      <c r="K557" s="2"/>
+      <c r="L557" s="2"/>
+      <c r="M557" s="2"/>
+    </row>
+    <row r="558" ht="15.75" customHeight="1">
+      <c r="A558" s="1">
+        <f t="shared" si="1"/>
+        <v>556</v>
+      </c>
+      <c r="B558" s="21">
+        <v>44477.0</v>
+      </c>
+      <c r="C558" s="2"/>
+      <c r="D558" s="2"/>
+      <c r="E558" s="2"/>
+      <c r="F558" s="2"/>
+      <c r="G558" s="2"/>
+      <c r="H558" s="2"/>
+      <c r="I558" s="2"/>
+      <c r="J558" s="2"/>
+      <c r="K558" s="2"/>
+      <c r="L558" s="2"/>
+      <c r="M558" s="2"/>
+    </row>
+    <row r="559" ht="15.75" customHeight="1">
+      <c r="A559" s="1">
+        <f t="shared" si="1"/>
+        <v>557</v>
+      </c>
+      <c r="B559" s="21">
+        <v>44478.0</v>
+      </c>
+      <c r="C559" s="2"/>
+      <c r="D559" s="2"/>
+      <c r="E559" s="2"/>
+      <c r="F559" s="2"/>
+      <c r="G559" s="2"/>
+      <c r="H559" s="2"/>
+      <c r="I559" s="2"/>
+      <c r="J559" s="2"/>
+      <c r="K559" s="2"/>
+      <c r="L559" s="2"/>
+      <c r="M559" s="2"/>
+    </row>
+    <row r="560" ht="15.75" customHeight="1">
+      <c r="A560" s="1">
+        <f t="shared" si="1"/>
+        <v>558</v>
+      </c>
+      <c r="B560" s="21">
+        <v>44479.0</v>
+      </c>
+      <c r="C560" s="2"/>
+      <c r="D560" s="2"/>
+      <c r="E560" s="2"/>
+      <c r="F560" s="2"/>
+      <c r="G560" s="2"/>
+      <c r="H560" s="2"/>
+      <c r="I560" s="2"/>
+      <c r="J560" s="2"/>
+      <c r="K560" s="2"/>
+      <c r="L560" s="2"/>
+      <c r="M560" s="2"/>
+    </row>
+    <row r="561" ht="15.75" customHeight="1">
+      <c r="A561" s="1">
+        <f t="shared" si="1"/>
+        <v>559</v>
+      </c>
+      <c r="B561" s="21">
+        <v>44480.0</v>
+      </c>
+      <c r="C561" s="2"/>
+      <c r="D561" s="2"/>
+      <c r="E561" s="2"/>
+      <c r="F561" s="2"/>
+      <c r="G561" s="2"/>
+      <c r="H561" s="2"/>
+      <c r="I561" s="2"/>
+      <c r="J561" s="2"/>
+      <c r="K561" s="2"/>
+      <c r="L561" s="2"/>
+      <c r="M561" s="2"/>
+    </row>
+    <row r="562" ht="15.75" customHeight="1">
+      <c r="A562" s="1">
+        <f t="shared" si="1"/>
+        <v>560</v>
+      </c>
+      <c r="B562" s="21">
+        <v>44481.0</v>
+      </c>
+      <c r="C562" s="2"/>
+      <c r="D562" s="2"/>
+      <c r="E562" s="2"/>
+      <c r="F562" s="2"/>
+      <c r="G562" s="2"/>
+      <c r="H562" s="2"/>
+      <c r="I562" s="2"/>
+      <c r="J562" s="2"/>
+      <c r="K562" s="2"/>
+      <c r="L562" s="2"/>
+      <c r="M562" s="2"/>
+    </row>
+    <row r="563" ht="15.75" customHeight="1">
+      <c r="A563" s="1">
+        <f t="shared" si="1"/>
+        <v>561</v>
+      </c>
+      <c r="B563" s="21">
+        <v>44482.0</v>
+      </c>
+      <c r="C563" s="2"/>
+      <c r="D563" s="2"/>
+      <c r="E563" s="2"/>
+      <c r="F563" s="2"/>
+      <c r="G563" s="2"/>
+      <c r="H563" s="2"/>
+      <c r="I563" s="2"/>
+      <c r="J563" s="2"/>
+      <c r="K563" s="2"/>
+      <c r="L563" s="2"/>
+      <c r="M563" s="2"/>
+    </row>
+    <row r="564" ht="15.75" customHeight="1">
+      <c r="A564" s="1">
+        <f t="shared" si="1"/>
+        <v>562</v>
+      </c>
+      <c r="B564" s="21">
+        <v>44483.0</v>
+      </c>
+      <c r="C564" s="2"/>
+      <c r="D564" s="2"/>
+      <c r="E564" s="2"/>
+      <c r="F564" s="2"/>
+      <c r="G564" s="2"/>
+      <c r="H564" s="2"/>
+      <c r="I564" s="2"/>
+      <c r="J564" s="2"/>
+      <c r="K564" s="2"/>
+      <c r="L564" s="2"/>
+      <c r="M564" s="2"/>
+    </row>
+    <row r="565" ht="15.75" customHeight="1">
+      <c r="A565" s="1">
+        <f t="shared" si="1"/>
+        <v>563</v>
+      </c>
+      <c r="B565" s="21">
+        <v>44484.0</v>
+      </c>
+      <c r="C565" s="2"/>
+      <c r="D565" s="2"/>
+      <c r="E565" s="2"/>
+      <c r="F565" s="2"/>
+      <c r="G565" s="2"/>
+      <c r="H565" s="2"/>
+      <c r="I565" s="2"/>
+      <c r="J565" s="2"/>
+      <c r="K565" s="2"/>
+      <c r="L565" s="2"/>
+      <c r="M565" s="2"/>
+    </row>
+    <row r="566" ht="15.75" customHeight="1">
+      <c r="A566" s="1">
+        <f t="shared" si="1"/>
+        <v>564</v>
+      </c>
+      <c r="B566" s="21">
+        <v>44485.0</v>
+      </c>
+      <c r="C566" s="2"/>
+      <c r="D566" s="2"/>
+      <c r="E566" s="2"/>
+      <c r="F566" s="2"/>
+      <c r="G566" s="2"/>
+      <c r="H566" s="2"/>
+      <c r="I566" s="2"/>
+      <c r="J566" s="2"/>
+      <c r="K566" s="2"/>
+      <c r="L566" s="2"/>
+      <c r="M566" s="2"/>
+    </row>
+    <row r="567" ht="15.75" customHeight="1">
+      <c r="A567" s="1">
+        <f t="shared" si="1"/>
+        <v>565</v>
+      </c>
+      <c r="B567" s="21">
+        <v>44486.0</v>
+      </c>
+      <c r="C567" s="2"/>
+      <c r="D567" s="2"/>
+      <c r="E567" s="2"/>
+      <c r="F567" s="2"/>
+      <c r="G567" s="2"/>
+      <c r="H567" s="2"/>
+      <c r="I567" s="2"/>
+      <c r="J567" s="2"/>
+      <c r="K567" s="2"/>
+      <c r="L567" s="2"/>
+      <c r="M567" s="2"/>
+    </row>
+    <row r="568" ht="15.75" customHeight="1">
+      <c r="A568" s="1">
+        <f t="shared" si="1"/>
+        <v>566</v>
+      </c>
+      <c r="B568" s="21">
+        <v>44487.0</v>
+      </c>
+      <c r="C568" s="2"/>
+      <c r="D568" s="2"/>
+      <c r="E568" s="2"/>
+      <c r="F568" s="2"/>
+      <c r="G568" s="2"/>
+      <c r="H568" s="2"/>
+      <c r="I568" s="2"/>
+      <c r="J568" s="2"/>
+      <c r="K568" s="2"/>
+      <c r="L568" s="2"/>
+      <c r="M568" s="2"/>
+    </row>
+    <row r="569" ht="15.75" customHeight="1">
+      <c r="A569" s="1">
+        <f t="shared" si="1"/>
+        <v>567</v>
+      </c>
+      <c r="B569" s="21">
+        <v>44488.0</v>
+      </c>
+      <c r="C569" s="2"/>
+      <c r="D569" s="2"/>
+      <c r="E569" s="2"/>
+      <c r="F569" s="2"/>
+      <c r="G569" s="2"/>
+      <c r="H569" s="2"/>
+      <c r="I569" s="2"/>
+      <c r="J569" s="2"/>
+      <c r="K569" s="2"/>
+      <c r="L569" s="2"/>
+      <c r="M569" s="2"/>
+    </row>
+    <row r="570" ht="15.75" customHeight="1">
+      <c r="A570" s="1">
+        <f t="shared" si="1"/>
+        <v>568</v>
+      </c>
+      <c r="B570" s="21">
+        <v>44489.0</v>
+      </c>
+      <c r="C570" s="2"/>
+      <c r="D570" s="2"/>
+      <c r="E570" s="2"/>
+      <c r="F570" s="2"/>
+      <c r="G570" s="2"/>
+      <c r="H570" s="2"/>
+      <c r="I570" s="2"/>
+      <c r="J570" s="2"/>
+      <c r="K570" s="2"/>
+      <c r="L570" s="2"/>
+      <c r="M570" s="2"/>
+    </row>
+    <row r="571" ht="15.75" customHeight="1">
+      <c r="A571" s="1">
+        <f t="shared" si="1"/>
+        <v>569</v>
+      </c>
+      <c r="B571" s="21">
+        <v>44490.0</v>
+      </c>
+      <c r="C571" s="2"/>
+      <c r="D571" s="2"/>
+      <c r="E571" s="2"/>
+      <c r="F571" s="2"/>
+      <c r="G571" s="2"/>
+      <c r="H571" s="2"/>
+      <c r="I571" s="2"/>
+      <c r="J571" s="2"/>
+      <c r="K571" s="2"/>
+      <c r="L571" s="2"/>
+      <c r="M571" s="2"/>
+    </row>
+    <row r="572" ht="15.75" customHeight="1">
+      <c r="A572" s="1">
+        <f t="shared" si="1"/>
+        <v>570</v>
+      </c>
+      <c r="B572" s="21">
+        <v>44491.0</v>
+      </c>
+      <c r="C572" s="2"/>
+      <c r="D572" s="2"/>
+      <c r="E572" s="2"/>
+      <c r="F572" s="2"/>
+      <c r="G572" s="2"/>
+      <c r="H572" s="2"/>
+      <c r="I572" s="2"/>
+      <c r="J572" s="2"/>
+      <c r="K572" s="2"/>
+      <c r="L572" s="2"/>
+      <c r="M572" s="2"/>
+    </row>
+    <row r="573" ht="15.75" customHeight="1">
+      <c r="A573" s="1">
+        <f t="shared" si="1"/>
+        <v>571</v>
+      </c>
+      <c r="B573" s="21">
+        <v>44492.0</v>
+      </c>
+      <c r="C573" s="2"/>
+      <c r="D573" s="2"/>
+      <c r="E573" s="2"/>
+      <c r="F573" s="2"/>
+      <c r="G573" s="2"/>
+      <c r="H573" s="2"/>
+      <c r="I573" s="2"/>
+      <c r="J573" s="2"/>
+      <c r="K573" s="2"/>
+      <c r="L573" s="2"/>
+      <c r="M573" s="2"/>
+    </row>
+    <row r="574" ht="15.75" customHeight="1">
+      <c r="A574" s="1">
+        <f t="shared" si="1"/>
+        <v>572</v>
+      </c>
+      <c r="B574" s="21">
+        <v>44493.0</v>
+      </c>
+      <c r="C574" s="2"/>
+      <c r="D574" s="2"/>
+      <c r="E574" s="2"/>
+      <c r="F574" s="2"/>
+      <c r="G574" s="2"/>
+      <c r="H574" s="2"/>
+      <c r="I574" s="2"/>
+      <c r="J574" s="2"/>
+      <c r="K574" s="2"/>
+      <c r="L574" s="2"/>
+      <c r="M574" s="2"/>
+    </row>
+    <row r="575" ht="15.75" customHeight="1">
+      <c r="A575" s="1">
+        <f t="shared" si="1"/>
+        <v>573</v>
+      </c>
+      <c r="B575" s="21">
+        <v>44494.0</v>
+      </c>
+      <c r="C575" s="2"/>
+      <c r="D575" s="2"/>
+      <c r="E575" s="2"/>
+      <c r="F575" s="2"/>
+      <c r="G575" s="2"/>
+      <c r="H575" s="2"/>
+      <c r="I575" s="2"/>
+      <c r="J575" s="2"/>
+      <c r="K575" s="2"/>
+      <c r="L575" s="2"/>
+      <c r="M575" s="2"/>
+    </row>
+    <row r="576" ht="15.75" customHeight="1">
+      <c r="A576" s="1">
+        <f t="shared" si="1"/>
+        <v>574</v>
+      </c>
+      <c r="B576" s="21">
+        <v>44495.0</v>
+      </c>
+      <c r="C576" s="2"/>
+      <c r="D576" s="2"/>
+      <c r="E576" s="2"/>
+      <c r="F576" s="2"/>
+      <c r="G576" s="2"/>
+      <c r="H576" s="2"/>
+      <c r="I576" s="2"/>
+      <c r="J576" s="2"/>
+      <c r="K576" s="2"/>
+      <c r="L576" s="2"/>
+      <c r="M576" s="2"/>
+    </row>
+    <row r="577" ht="15.75" customHeight="1">
+      <c r="A577" s="1">
+        <f t="shared" si="1"/>
+        <v>575</v>
+      </c>
+      <c r="B577" s="21">
+        <v>44496.0</v>
+      </c>
+      <c r="C577" s="2"/>
+      <c r="D577" s="2"/>
+      <c r="E577" s="2"/>
+      <c r="F577" s="2"/>
+      <c r="G577" s="2"/>
+      <c r="H577" s="2"/>
+      <c r="I577" s="2"/>
+      <c r="J577" s="2"/>
+      <c r="K577" s="2"/>
+      <c r="L577" s="2"/>
+      <c r="M577" s="2"/>
+    </row>
+    <row r="578" ht="15.75" customHeight="1">
+      <c r="A578" s="1">
+        <f t="shared" si="1"/>
+        <v>576</v>
+      </c>
+      <c r="B578" s="21">
+        <v>44497.0</v>
+      </c>
+      <c r="C578" s="2"/>
+      <c r="D578" s="2"/>
+      <c r="E578" s="2"/>
+      <c r="F578" s="2"/>
+      <c r="G578" s="2"/>
+      <c r="H578" s="2"/>
+      <c r="I578" s="2"/>
+      <c r="J578" s="2"/>
+      <c r="K578" s="2"/>
+      <c r="L578" s="2"/>
+      <c r="M578" s="2"/>
+    </row>
+    <row r="579" ht="15.75" customHeight="1">
+      <c r="A579" s="1">
+        <f t="shared" si="1"/>
+        <v>577</v>
+      </c>
+      <c r="B579" s="21">
+        <v>44498.0</v>
+      </c>
+      <c r="C579" s="2"/>
+      <c r="D579" s="2"/>
+      <c r="E579" s="2"/>
+      <c r="F579" s="2"/>
+      <c r="G579" s="2"/>
+      <c r="H579" s="2"/>
+      <c r="I579" s="2"/>
+      <c r="J579" s="2"/>
+      <c r="K579" s="2"/>
+      <c r="L579" s="2"/>
+      <c r="M579" s="2"/>
+    </row>
+    <row r="580" ht="15.75" customHeight="1">
+      <c r="A580" s="1">
+        <f t="shared" si="1"/>
+        <v>578</v>
+      </c>
+      <c r="B580" s="21">
+        <v>44499.0</v>
+      </c>
+      <c r="C580" s="2"/>
+      <c r="D580" s="2"/>
+      <c r="E580" s="2"/>
+      <c r="F580" s="2"/>
+      <c r="G580" s="2"/>
+      <c r="H580" s="2"/>
+      <c r="I580" s="2"/>
+      <c r="J580" s="2"/>
+      <c r="K580" s="2"/>
+      <c r="L580" s="2"/>
+      <c r="M580" s="2"/>
+    </row>
+    <row r="581" ht="15.75" customHeight="1">
+      <c r="A581" s="1">
+        <f t="shared" si="1"/>
+        <v>579</v>
+      </c>
+      <c r="B581" s="21">
+        <v>44500.0</v>
+      </c>
+      <c r="C581" s="2"/>
+      <c r="D581" s="2"/>
+      <c r="E581" s="2"/>
+      <c r="F581" s="2"/>
+      <c r="G581" s="2"/>
+      <c r="H581" s="2"/>
+      <c r="I581" s="2"/>
+      <c r="J581" s="2"/>
+      <c r="K581" s="2"/>
+      <c r="L581" s="2"/>
+      <c r="M581" s="2"/>
+    </row>
+    <row r="582" ht="15.75" customHeight="1">
+      <c r="A582" s="19"/>
+    </row>
     <row r="583" ht="15.75" customHeight="1"/>
     <row r="584" ht="15.75" customHeight="1"/>
     <row r="585" ht="15.75" customHeight="1"/>
@@ -18684,7 +19611,7 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{88A7EE37-FF51-4D26-B0DB-7723BB5C1D1C}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{B5C5D958-6324-40D8-B4E1-76BBA7389C94}" filter="1" showAutoFilter="1">
       <autoFilter ref="$G$9"/>
       <extLst>
         <ext uri="GoogleSheetsCustomDataVersion1">

</xml_diff>

<commit_message>
Added data on 10 Oct
</commit_message>
<xml_diff>
--- a/Araraquara_covid.xlsx
+++ b/Araraquara_covid.xlsx
@@ -6,11 +6,11 @@
     <sheet state="visible" name="Araraquara covid.csv" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="Z_B5C5D958_6324_40D8_B4E1_76BBA7389C94_.wvu.FilterData">'Araraquara covid.csv'!$G$9</definedName>
+    <definedName hidden="1" localSheetId="0" name="Z_D43912C3_DA06_41C2_8E8C_8C4107953FBA_.wvu.FilterData">'Araraquara covid.csv'!$G$9</definedName>
   </definedNames>
   <calcPr/>
   <customWorkbookViews>
-    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{B5C5D958-6324-40D8-B4E1-76BBA7389C94}" name="Filtro 1"/>
+    <customWorkbookView activeSheetId="0" maximized="1" windowHeight="0" windowWidth="0" guid="{D43912C3-DA06-41C2-8E8C-8C4107953FBA}" name="Filtro 1"/>
   </customWorkbookViews>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
@@ -123,7 +123,7 @@
   </commentList>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mhsCv6ErEnzZl9lc9UDQB1vUrdLhw=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId1" roundtripDataSignature="AMtx7mjh5M2JocVpcEKsouFieT0vYWv57w=="/>
     </ext>
   </extLst>
 </comments>
@@ -260,7 +260,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="20">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -319,12 +319,6 @@
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="6" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -644,7 +638,7 @@
         <v>5.0</v>
       </c>
       <c r="D3" s="2">
-        <f t="shared" ref="D3:D552" si="2">(C3-C2)</f>
+        <f t="shared" ref="D3:D560" si="2">(C3-C2)</f>
         <v>2</v>
       </c>
       <c r="E3" s="1">
@@ -18014,38 +18008,38 @@
       <c r="B539" s="5">
         <v>44458.0</v>
       </c>
-      <c r="C539" s="19">
+      <c r="C539" s="1">
         <v>29951.0</v>
       </c>
       <c r="D539" s="2">
         <f t="shared" si="2"/>
         <v>34</v>
       </c>
-      <c r="E539" s="19">
+      <c r="E539" s="1">
         <v>584.0</v>
       </c>
-      <c r="F539" s="19">
+      <c r="F539" s="1">
         <v>18.0</v>
       </c>
-      <c r="G539" s="19">
+      <c r="G539" s="1">
         <v>17.0</v>
       </c>
-      <c r="H539" s="19">
+      <c r="H539" s="1">
         <v>5.0</v>
       </c>
-      <c r="I539" s="19">
+      <c r="I539" s="1">
         <v>192410.0</v>
       </c>
-      <c r="J539" s="19">
+      <c r="J539" s="1">
         <v>125022.0</v>
       </c>
-      <c r="K539" s="19">
-        <v>0.0</v>
-      </c>
-      <c r="L539" s="19">
+      <c r="K539" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="L539" s="1">
         <v>890.0</v>
       </c>
-      <c r="M539" s="19">
+      <c r="M539" s="1">
         <v>318322.0</v>
       </c>
     </row>
@@ -18057,38 +18051,38 @@
       <c r="B540" s="5">
         <v>44459.0</v>
       </c>
-      <c r="C540" s="19">
+      <c r="C540" s="1">
         <v>29956.0</v>
       </c>
       <c r="D540" s="2">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="E540" s="19">
+      <c r="E540" s="1">
         <v>584.0</v>
       </c>
-      <c r="F540" s="19">
+      <c r="F540" s="1">
         <v>18.0</v>
       </c>
-      <c r="G540" s="19">
+      <c r="G540" s="1">
         <v>17.0</v>
       </c>
-      <c r="H540" s="19">
+      <c r="H540" s="1">
         <v>5.0</v>
       </c>
-      <c r="I540" s="19">
+      <c r="I540" s="1">
         <v>192472.0</v>
       </c>
-      <c r="J540" s="19">
+      <c r="J540" s="1">
         <v>125409.0</v>
       </c>
-      <c r="K540" s="19">
-        <v>0.0</v>
-      </c>
-      <c r="L540" s="19">
+      <c r="K540" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="L540" s="1">
         <v>900.0</v>
       </c>
-      <c r="M540" s="19">
+      <c r="M540" s="1">
         <v>318781.0</v>
       </c>
     </row>
@@ -18100,38 +18094,38 @@
       <c r="B541" s="5">
         <v>44460.0</v>
       </c>
-      <c r="C541" s="19">
+      <c r="C541" s="1">
         <v>30014.0</v>
       </c>
       <c r="D541" s="2">
         <f t="shared" si="2"/>
         <v>58</v>
       </c>
-      <c r="E541" s="19">
+      <c r="E541" s="1">
         <v>584.0</v>
       </c>
-      <c r="F541" s="19">
+      <c r="F541" s="1">
         <v>17.0</v>
       </c>
-      <c r="G541" s="19">
+      <c r="G541" s="1">
         <v>16.0</v>
       </c>
-      <c r="H541" s="19">
+      <c r="H541" s="1">
         <v>5.0</v>
       </c>
-      <c r="I541" s="19">
+      <c r="I541" s="1">
         <v>192943.0</v>
       </c>
-      <c r="J541" s="19">
+      <c r="J541" s="1">
         <v>127253.0</v>
       </c>
-      <c r="K541" s="19">
-        <v>0.0</v>
-      </c>
-      <c r="L541" s="19">
+      <c r="K541" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="L541" s="1">
         <v>979.0</v>
       </c>
-      <c r="M541" s="19">
+      <c r="M541" s="1">
         <v>321175.0</v>
       </c>
     </row>
@@ -18143,38 +18137,38 @@
       <c r="B542" s="5">
         <v>44461.0</v>
       </c>
-      <c r="C542" s="19">
+      <c r="C542" s="1">
         <v>30053.0</v>
       </c>
       <c r="D542" s="2">
         <f t="shared" si="2"/>
         <v>39</v>
       </c>
-      <c r="E542" s="19">
+      <c r="E542" s="1">
         <v>584.0</v>
       </c>
-      <c r="F542" s="19">
+      <c r="F542" s="1">
         <v>17.0</v>
       </c>
-      <c r="G542" s="19">
+      <c r="G542" s="1">
         <v>16.0</v>
       </c>
-      <c r="H542" s="19">
+      <c r="H542" s="1">
         <v>4.0</v>
       </c>
-      <c r="I542" s="19">
+      <c r="I542" s="1">
         <v>193302.0</v>
       </c>
-      <c r="J542" s="19">
+      <c r="J542" s="1">
         <v>129966.0</v>
       </c>
-      <c r="K542" s="19">
-        <v>0.0</v>
-      </c>
-      <c r="L542" s="19">
+      <c r="K542" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="L542" s="1">
         <v>1129.0</v>
       </c>
-      <c r="M542" s="19">
+      <c r="M542" s="1">
         <v>324397.0</v>
       </c>
     </row>
@@ -18186,38 +18180,38 @@
       <c r="B543" s="5">
         <v>44462.0</v>
       </c>
-      <c r="C543" s="19">
+      <c r="C543" s="1">
         <v>30115.0</v>
       </c>
       <c r="D543" s="2">
         <f t="shared" si="2"/>
         <v>62</v>
       </c>
-      <c r="E543" s="19">
+      <c r="E543" s="1">
         <v>584.0</v>
       </c>
-      <c r="F543" s="19">
+      <c r="F543" s="1">
         <v>14.0</v>
       </c>
-      <c r="G543" s="19">
+      <c r="G543" s="1">
         <v>14.0</v>
       </c>
-      <c r="H543" s="19">
+      <c r="H543" s="1">
         <v>4.0</v>
       </c>
-      <c r="I543" s="19">
+      <c r="I543" s="1">
         <v>193558.0</v>
       </c>
-      <c r="J543" s="19">
+      <c r="J543" s="1">
         <v>132558.0</v>
       </c>
-      <c r="K543" s="19">
-        <v>0.0</v>
-      </c>
-      <c r="L543" s="19">
+      <c r="K543" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="L543" s="1">
         <v>1408.0</v>
       </c>
-      <c r="M543" s="19">
+      <c r="M543" s="1">
         <v>327524.0</v>
       </c>
     </row>
@@ -18229,38 +18223,38 @@
       <c r="B544" s="5">
         <v>44463.0</v>
       </c>
-      <c r="C544" s="19">
+      <c r="C544" s="1">
         <v>30144.0</v>
       </c>
       <c r="D544" s="2">
         <f t="shared" si="2"/>
         <v>29</v>
       </c>
-      <c r="E544" s="19">
+      <c r="E544" s="1">
         <v>584.0</v>
       </c>
-      <c r="F544" s="19">
+      <c r="F544" s="1">
         <v>18.0</v>
       </c>
-      <c r="G544" s="19">
+      <c r="G544" s="1">
         <v>16.0</v>
       </c>
-      <c r="H544" s="19">
+      <c r="H544" s="1">
         <v>8.0</v>
       </c>
-      <c r="I544" s="19">
+      <c r="I544" s="1">
         <v>193860.0</v>
       </c>
-      <c r="J544" s="19">
+      <c r="J544" s="1">
         <v>135291.0</v>
       </c>
-      <c r="K544" s="19">
-        <v>0.0</v>
-      </c>
-      <c r="L544" s="19">
+      <c r="K544" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="L544" s="1">
         <v>1512.0</v>
       </c>
-      <c r="M544" s="19">
+      <c r="M544" s="1">
         <v>330663.0</v>
       </c>
     </row>
@@ -18272,38 +18266,38 @@
       <c r="B545" s="5">
         <v>44464.0</v>
       </c>
-      <c r="C545" s="19">
+      <c r="C545" s="1">
         <v>30186.0</v>
       </c>
       <c r="D545" s="2">
         <f t="shared" si="2"/>
         <v>42</v>
       </c>
-      <c r="E545" s="19">
+      <c r="E545" s="1">
         <v>584.0</v>
       </c>
-      <c r="F545" s="19">
+      <c r="F545" s="1">
         <v>15.0</v>
       </c>
-      <c r="G545" s="19">
+      <c r="G545" s="1">
         <v>14.0</v>
       </c>
-      <c r="H545" s="19">
+      <c r="H545" s="1">
         <v>7.0</v>
       </c>
-      <c r="I545" s="19">
+      <c r="I545" s="1">
         <v>194056.0</v>
       </c>
-      <c r="J545" s="19">
+      <c r="J545" s="1">
         <v>138108.0</v>
       </c>
-      <c r="K545" s="19">
-        <v>0.0</v>
-      </c>
-      <c r="L545" s="19">
+      <c r="K545" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="L545" s="1">
         <v>1681.0</v>
       </c>
-      <c r="M545" s="19">
+      <c r="M545" s="1">
         <v>333845.0</v>
       </c>
     </row>
@@ -18315,38 +18309,38 @@
       <c r="B546" s="5">
         <v>44465.0</v>
       </c>
-      <c r="C546" s="19">
+      <c r="C546" s="1">
         <v>30224.0</v>
       </c>
       <c r="D546" s="2">
         <f t="shared" si="2"/>
         <v>38</v>
       </c>
-      <c r="E546" s="19">
+      <c r="E546" s="1">
         <v>585.0</v>
       </c>
-      <c r="F546" s="19">
+      <c r="F546" s="1">
         <v>17.0</v>
       </c>
-      <c r="G546" s="19">
+      <c r="G546" s="1">
         <v>14.0</v>
       </c>
-      <c r="H546" s="19">
+      <c r="H546" s="1">
         <v>7.0</v>
       </c>
-      <c r="I546" s="19">
+      <c r="I546" s="1">
         <v>194187.0</v>
       </c>
-      <c r="J546" s="19">
+      <c r="J546" s="1">
         <v>139779.0</v>
       </c>
-      <c r="K546" s="19">
-        <v>0.0</v>
-      </c>
-      <c r="L546" s="19">
+      <c r="K546" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="L546" s="1">
         <v>1770.0</v>
       </c>
-      <c r="M546" s="19">
+      <c r="M546" s="1">
         <v>335736.0</v>
       </c>
     </row>
@@ -18358,38 +18352,38 @@
       <c r="B547" s="5">
         <v>44466.0</v>
       </c>
-      <c r="C547" s="19">
+      <c r="C547" s="1">
         <v>30237.0</v>
       </c>
       <c r="D547" s="2">
         <f t="shared" si="2"/>
         <v>13</v>
       </c>
-      <c r="E547" s="19">
+      <c r="E547" s="1">
         <v>586.0</v>
       </c>
-      <c r="F547" s="19">
+      <c r="F547" s="1">
         <v>19.0</v>
       </c>
-      <c r="G547" s="19">
+      <c r="G547" s="1">
         <v>15.0</v>
       </c>
-      <c r="H547" s="19">
+      <c r="H547" s="1">
         <v>7.0</v>
       </c>
-      <c r="I547" s="19">
+      <c r="I547" s="1">
         <v>194191.0</v>
       </c>
-      <c r="J547" s="20">
+      <c r="J547" s="15">
         <v>139794.0</v>
       </c>
-      <c r="K547" s="19">
+      <c r="K547" s="1">
         <v>0.0</v>
       </c>
       <c r="L547" s="16">
         <v>1770.0</v>
       </c>
-      <c r="M547" s="19">
+      <c r="M547" s="1">
         <v>335755.0</v>
       </c>
     </row>
@@ -18401,38 +18395,38 @@
       <c r="B548" s="5">
         <v>44467.0</v>
       </c>
-      <c r="C548" s="19">
+      <c r="C548" s="1">
         <v>30270.0</v>
       </c>
       <c r="D548" s="2">
         <f t="shared" si="2"/>
         <v>33</v>
       </c>
-      <c r="E548" s="19">
+      <c r="E548" s="1">
         <v>586.0</v>
       </c>
-      <c r="F548" s="19">
+      <c r="F548" s="1">
         <v>19.0</v>
       </c>
-      <c r="G548" s="19">
+      <c r="G548" s="1">
         <v>16.0</v>
       </c>
-      <c r="H548" s="19">
+      <c r="H548" s="1">
         <v>7.0</v>
       </c>
-      <c r="I548" s="19">
+      <c r="I548" s="1">
         <v>194366.0</v>
       </c>
-      <c r="J548" s="19">
+      <c r="J548" s="1">
         <v>141731.0</v>
       </c>
-      <c r="K548" s="19">
-        <v>0.0</v>
-      </c>
-      <c r="L548" s="19">
+      <c r="K548" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="L548" s="1">
         <v>1796.0</v>
       </c>
-      <c r="M548" s="19">
+      <c r="M548" s="1">
         <v>337893.0</v>
       </c>
     </row>
@@ -18444,38 +18438,38 @@
       <c r="B549" s="5">
         <v>44468.0</v>
       </c>
-      <c r="C549" s="19">
+      <c r="C549" s="1">
         <v>30298.0</v>
       </c>
       <c r="D549" s="2">
         <f t="shared" si="2"/>
         <v>28</v>
       </c>
-      <c r="E549" s="19">
+      <c r="E549" s="1">
         <v>586.0</v>
       </c>
-      <c r="F549" s="19">
+      <c r="F549" s="1">
         <v>19.0</v>
       </c>
-      <c r="G549" s="19">
+      <c r="G549" s="1">
         <v>17.0</v>
       </c>
-      <c r="H549" s="19">
+      <c r="H549" s="1">
         <v>6.0</v>
       </c>
-      <c r="I549" s="19">
+      <c r="I549" s="1">
         <v>194690.0</v>
       </c>
-      <c r="J549" s="19">
+      <c r="J549" s="1">
         <v>145463.0</v>
       </c>
-      <c r="K549" s="19">
-        <v>0.0</v>
-      </c>
-      <c r="L549" s="19">
+      <c r="K549" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="L549" s="1">
         <v>1939.0</v>
       </c>
-      <c r="M549" s="19">
+      <c r="M549" s="1">
         <v>342092.0</v>
       </c>
     </row>
@@ -18487,38 +18481,38 @@
       <c r="B550" s="5">
         <v>44469.0</v>
       </c>
-      <c r="C550" s="19">
+      <c r="C550" s="1">
         <v>30328.0</v>
       </c>
       <c r="D550" s="2">
         <f t="shared" si="2"/>
         <v>30</v>
       </c>
-      <c r="E550" s="19">
+      <c r="E550" s="1">
         <v>586.0</v>
       </c>
-      <c r="F550" s="19">
+      <c r="F550" s="1">
         <v>18.0</v>
       </c>
-      <c r="G550" s="19">
+      <c r="G550" s="1">
         <v>15.0</v>
       </c>
-      <c r="H550" s="19">
+      <c r="H550" s="1">
         <v>8.0</v>
       </c>
-      <c r="I550" s="19">
+      <c r="I550" s="1">
         <v>195016.0</v>
       </c>
-      <c r="J550" s="19">
+      <c r="J550" s="1">
         <v>148922.0</v>
       </c>
-      <c r="K550" s="19">
-        <v>0.0</v>
-      </c>
-      <c r="L550" s="19">
+      <c r="K550" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="L550" s="1">
         <v>2136.0</v>
       </c>
-      <c r="M550" s="19">
+      <c r="M550" s="1">
         <v>346074.0</v>
       </c>
     </row>
@@ -18527,41 +18521,41 @@
         <f t="shared" si="1"/>
         <v>549</v>
       </c>
-      <c r="B551" s="21">
+      <c r="B551" s="5">
         <v>44470.0</v>
       </c>
-      <c r="C551" s="19">
+      <c r="C551" s="1">
         <v>30347.0</v>
       </c>
       <c r="D551" s="2">
         <f t="shared" si="2"/>
         <v>19</v>
       </c>
-      <c r="E551" s="19">
+      <c r="E551" s="1">
         <v>586.0</v>
       </c>
-      <c r="F551" s="19">
+      <c r="F551" s="1">
         <v>20.0</v>
       </c>
-      <c r="G551" s="19">
+      <c r="G551" s="1">
         <v>18.0</v>
       </c>
-      <c r="H551" s="19">
+      <c r="H551" s="1">
         <v>8.0</v>
       </c>
-      <c r="I551" s="19">
+      <c r="I551" s="1">
         <v>195272.0</v>
       </c>
-      <c r="J551" s="19">
+      <c r="J551" s="1">
         <v>150761.0</v>
       </c>
-      <c r="K551" s="19">
-        <v>0.0</v>
-      </c>
-      <c r="L551" s="19">
+      <c r="K551" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="L551" s="1">
         <v>2290.0</v>
       </c>
-      <c r="M551" s="19">
+      <c r="M551" s="1">
         <v>348323.0</v>
       </c>
     </row>
@@ -18570,41 +18564,41 @@
         <f t="shared" si="1"/>
         <v>550</v>
       </c>
-      <c r="B552" s="21">
+      <c r="B552" s="5">
         <v>44471.0</v>
       </c>
-      <c r="C552" s="19">
+      <c r="C552" s="1">
         <v>30366.0</v>
       </c>
       <c r="D552" s="2">
         <f t="shared" si="2"/>
         <v>19</v>
       </c>
-      <c r="E552" s="19">
+      <c r="E552" s="1">
         <v>586.0</v>
       </c>
-      <c r="F552" s="19">
+      <c r="F552" s="1">
         <v>18.0</v>
       </c>
-      <c r="G552" s="19">
+      <c r="G552" s="1">
         <v>18.0</v>
       </c>
-      <c r="H552" s="19">
+      <c r="H552" s="1">
         <v>9.0</v>
       </c>
-      <c r="I552" s="19">
+      <c r="I552" s="1">
         <v>195552.0</v>
       </c>
-      <c r="J552" s="19">
+      <c r="J552" s="1">
         <v>152424.0</v>
       </c>
-      <c r="K552" s="19">
-        <v>0.0</v>
-      </c>
-      <c r="L552" s="19">
+      <c r="K552" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="L552" s="1">
         <v>2375.0</v>
       </c>
-      <c r="M552" s="19">
+      <c r="M552" s="1">
         <v>350351.0</v>
       </c>
     </row>
@@ -18613,167 +18607,351 @@
         <f t="shared" si="1"/>
         <v>551</v>
       </c>
-      <c r="B553" s="21">
+      <c r="B553" s="5">
         <v>44472.0</v>
       </c>
-      <c r="C553" s="2"/>
-      <c r="D553" s="2"/>
-      <c r="E553" s="2"/>
-      <c r="F553" s="2"/>
-      <c r="G553" s="2"/>
-      <c r="H553" s="2"/>
-      <c r="I553" s="2"/>
-      <c r="J553" s="2"/>
-      <c r="K553" s="2"/>
-      <c r="L553" s="2"/>
-      <c r="M553" s="2"/>
+      <c r="C553" s="1">
+        <v>30381.0</v>
+      </c>
+      <c r="D553" s="2">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="E553" s="1">
+        <v>588.0</v>
+      </c>
+      <c r="F553" s="1">
+        <v>15.0</v>
+      </c>
+      <c r="G553" s="1">
+        <v>13.0</v>
+      </c>
+      <c r="H553" s="1">
+        <v>7.0</v>
+      </c>
+      <c r="I553" s="1">
+        <v>195786.0</v>
+      </c>
+      <c r="J553" s="1">
+        <v>153544.0</v>
+      </c>
+      <c r="K553" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="L553" s="1">
+        <v>2409.0</v>
+      </c>
+      <c r="M553" s="1">
+        <v>351739.0</v>
+      </c>
     </row>
     <row r="554" ht="15.75" customHeight="1">
       <c r="A554" s="1">
         <f t="shared" si="1"/>
         <v>552</v>
       </c>
-      <c r="B554" s="21">
+      <c r="B554" s="5">
         <v>44473.0</v>
       </c>
-      <c r="C554" s="2"/>
-      <c r="D554" s="2"/>
-      <c r="E554" s="2"/>
-      <c r="F554" s="2"/>
-      <c r="G554" s="2"/>
-      <c r="H554" s="2"/>
-      <c r="I554" s="2"/>
-      <c r="J554" s="2"/>
-      <c r="K554" s="2"/>
-      <c r="L554" s="2"/>
-      <c r="M554" s="2"/>
+      <c r="C554" s="1">
+        <v>30382.0</v>
+      </c>
+      <c r="D554" s="2">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="E554" s="1">
+        <v>588.0</v>
+      </c>
+      <c r="F554" s="1">
+        <v>15.0</v>
+      </c>
+      <c r="G554" s="1">
+        <v>12.0</v>
+      </c>
+      <c r="H554" s="1">
+        <v>7.0</v>
+      </c>
+      <c r="I554" s="1">
+        <v>195865.0</v>
+      </c>
+      <c r="J554" s="1">
+        <v>153780.0</v>
+      </c>
+      <c r="K554" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="L554" s="1">
+        <v>2413.0</v>
+      </c>
+      <c r="M554" s="1">
+        <v>352058.0</v>
+      </c>
     </row>
     <row r="555" ht="15.75" customHeight="1">
       <c r="A555" s="1">
         <f t="shared" si="1"/>
         <v>553</v>
       </c>
-      <c r="B555" s="21">
+      <c r="B555" s="5">
         <v>44474.0</v>
       </c>
-      <c r="C555" s="2"/>
-      <c r="D555" s="2"/>
-      <c r="E555" s="2"/>
-      <c r="F555" s="2"/>
-      <c r="G555" s="2"/>
-      <c r="H555" s="2"/>
-      <c r="I555" s="2"/>
-      <c r="J555" s="2"/>
-      <c r="K555" s="2"/>
-      <c r="L555" s="2"/>
-      <c r="M555" s="2"/>
+      <c r="C555" s="1">
+        <v>30398.0</v>
+      </c>
+      <c r="D555" s="2">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="E555" s="1">
+        <v>589.0</v>
+      </c>
+      <c r="F555" s="1">
+        <v>10.0</v>
+      </c>
+      <c r="G555" s="1">
+        <v>9.0</v>
+      </c>
+      <c r="H555" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="I555" s="1">
+        <v>196053.0</v>
+      </c>
+      <c r="J555" s="1">
+        <v>154834.0</v>
+      </c>
+      <c r="K555" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="L555" s="1">
+        <v>2467.0</v>
+      </c>
+      <c r="M555" s="1">
+        <v>353354.0</v>
+      </c>
     </row>
     <row r="556" ht="15.75" customHeight="1">
       <c r="A556" s="1">
         <f t="shared" si="1"/>
         <v>554</v>
       </c>
-      <c r="B556" s="21">
+      <c r="B556" s="5">
         <v>44475.0</v>
       </c>
-      <c r="C556" s="2"/>
-      <c r="D556" s="2"/>
-      <c r="E556" s="2"/>
-      <c r="F556" s="2"/>
-      <c r="G556" s="2"/>
-      <c r="H556" s="2"/>
-      <c r="I556" s="2"/>
-      <c r="J556" s="2"/>
-      <c r="K556" s="2"/>
-      <c r="L556" s="2"/>
-      <c r="M556" s="2"/>
+      <c r="C556" s="1">
+        <v>30424.0</v>
+      </c>
+      <c r="D556" s="2">
+        <f t="shared" si="2"/>
+        <v>26</v>
+      </c>
+      <c r="E556" s="1">
+        <v>589.0</v>
+      </c>
+      <c r="F556" s="1">
+        <v>10.0</v>
+      </c>
+      <c r="G556" s="1">
+        <v>9.0</v>
+      </c>
+      <c r="H556" s="1">
+        <v>6.0</v>
+      </c>
+      <c r="I556" s="1">
+        <v>196251.0</v>
+      </c>
+      <c r="J556" s="1">
+        <v>156712.0</v>
+      </c>
+      <c r="K556" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="L556" s="1">
+        <v>2592.0</v>
+      </c>
+      <c r="M556" s="1">
+        <v>355555.0</v>
+      </c>
     </row>
     <row r="557" ht="15.75" customHeight="1">
       <c r="A557" s="1">
         <f t="shared" si="1"/>
         <v>555</v>
       </c>
-      <c r="B557" s="21">
+      <c r="B557" s="5">
         <v>44476.0</v>
       </c>
-      <c r="C557" s="2"/>
-      <c r="D557" s="2"/>
-      <c r="E557" s="2"/>
-      <c r="F557" s="2"/>
-      <c r="G557" s="2"/>
-      <c r="H557" s="2"/>
-      <c r="I557" s="2"/>
-      <c r="J557" s="2"/>
-      <c r="K557" s="2"/>
-      <c r="L557" s="2"/>
-      <c r="M557" s="2"/>
+      <c r="C557" s="1">
+        <v>30436.0</v>
+      </c>
+      <c r="D557" s="2">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="E557" s="1">
+        <v>591.0</v>
+      </c>
+      <c r="F557" s="1">
+        <v>10.0</v>
+      </c>
+      <c r="G557" s="1">
+        <v>9.0</v>
+      </c>
+      <c r="H557" s="1">
+        <v>5.0</v>
+      </c>
+      <c r="I557" s="1">
+        <v>196429.0</v>
+      </c>
+      <c r="J557" s="1">
+        <v>157796.0</v>
+      </c>
+      <c r="K557" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="L557" s="1">
+        <v>3245.0</v>
+      </c>
+      <c r="M557" s="1">
+        <v>357470.0</v>
+      </c>
     </row>
     <row r="558" ht="15.75" customHeight="1">
       <c r="A558" s="1">
         <f t="shared" si="1"/>
         <v>556</v>
       </c>
-      <c r="B558" s="21">
+      <c r="B558" s="5">
         <v>44477.0</v>
       </c>
-      <c r="C558" s="2"/>
-      <c r="D558" s="2"/>
-      <c r="E558" s="2"/>
-      <c r="F558" s="2"/>
-      <c r="G558" s="2"/>
-      <c r="H558" s="2"/>
-      <c r="I558" s="2"/>
-      <c r="J558" s="2"/>
-      <c r="K558" s="2"/>
-      <c r="L558" s="2"/>
-      <c r="M558" s="2"/>
+      <c r="C558" s="19">
+        <v>30452.0</v>
+      </c>
+      <c r="D558" s="2">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="E558" s="19">
+        <v>591.0</v>
+      </c>
+      <c r="F558" s="19">
+        <v>10.0</v>
+      </c>
+      <c r="G558" s="19">
+        <v>10.0</v>
+      </c>
+      <c r="H558" s="19">
+        <v>4.0</v>
+      </c>
+      <c r="I558" s="19">
+        <v>196594.0</v>
+      </c>
+      <c r="J558" s="19">
+        <v>158830.0</v>
+      </c>
+      <c r="K558" s="19">
+        <v>0.0</v>
+      </c>
+      <c r="L558" s="19">
+        <v>4087.0</v>
+      </c>
+      <c r="M558" s="19">
+        <v>359511.0</v>
+      </c>
     </row>
     <row r="559" ht="15.75" customHeight="1">
       <c r="A559" s="1">
         <f t="shared" si="1"/>
         <v>557</v>
       </c>
-      <c r="B559" s="21">
+      <c r="B559" s="5">
         <v>44478.0</v>
       </c>
-      <c r="C559" s="2"/>
-      <c r="D559" s="2"/>
-      <c r="E559" s="2"/>
-      <c r="F559" s="2"/>
-      <c r="G559" s="2"/>
-      <c r="H559" s="2"/>
-      <c r="I559" s="2"/>
-      <c r="J559" s="2"/>
-      <c r="K559" s="2"/>
-      <c r="L559" s="2"/>
-      <c r="M559" s="2"/>
+      <c r="C559" s="19">
+        <v>30463.0</v>
+      </c>
+      <c r="D559" s="2">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="E559" s="19">
+        <v>592.0</v>
+      </c>
+      <c r="F559" s="19">
+        <v>9.0</v>
+      </c>
+      <c r="G559" s="19">
+        <v>9.0</v>
+      </c>
+      <c r="H559" s="19">
+        <v>6.0</v>
+      </c>
+      <c r="I559" s="19">
+        <v>196742.0</v>
+      </c>
+      <c r="J559" s="19">
+        <v>160076.0</v>
+      </c>
+      <c r="K559" s="19">
+        <v>0.0</v>
+      </c>
+      <c r="L559" s="19">
+        <v>4547.0</v>
+      </c>
+      <c r="M559" s="19">
+        <v>361365.0</v>
+      </c>
     </row>
     <row r="560" ht="15.75" customHeight="1">
       <c r="A560" s="1">
         <f t="shared" si="1"/>
         <v>558</v>
       </c>
-      <c r="B560" s="21">
+      <c r="B560" s="5">
         <v>44479.0</v>
       </c>
-      <c r="C560" s="2"/>
-      <c r="D560" s="2"/>
-      <c r="E560" s="2"/>
-      <c r="F560" s="2"/>
-      <c r="G560" s="2"/>
-      <c r="H560" s="2"/>
-      <c r="I560" s="2"/>
-      <c r="J560" s="2"/>
-      <c r="K560" s="2"/>
-      <c r="L560" s="2"/>
-      <c r="M560" s="2"/>
+      <c r="C560" s="19">
+        <v>30470.0</v>
+      </c>
+      <c r="D560" s="2">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="E560" s="19">
+        <v>592.0</v>
+      </c>
+      <c r="F560" s="19">
+        <v>13.0</v>
+      </c>
+      <c r="G560" s="19">
+        <v>13.0</v>
+      </c>
+      <c r="H560" s="19">
+        <v>7.0</v>
+      </c>
+      <c r="I560" s="19">
+        <v>196742.0</v>
+      </c>
+      <c r="J560" s="19">
+        <v>160077.0</v>
+      </c>
+      <c r="K560" s="19">
+        <v>0.0</v>
+      </c>
+      <c r="L560" s="19">
+        <v>4559.0</v>
+      </c>
+      <c r="M560" s="19">
+        <v>361378.0</v>
+      </c>
     </row>
     <row r="561" ht="15.75" customHeight="1">
       <c r="A561" s="1">
         <f t="shared" si="1"/>
         <v>559</v>
       </c>
-      <c r="B561" s="21">
+      <c r="B561" s="5">
         <v>44480.0</v>
       </c>
       <c r="C561" s="2"/>
@@ -18793,7 +18971,7 @@
         <f t="shared" si="1"/>
         <v>560</v>
       </c>
-      <c r="B562" s="21">
+      <c r="B562" s="5">
         <v>44481.0</v>
       </c>
       <c r="C562" s="2"/>
@@ -18813,7 +18991,7 @@
         <f t="shared" si="1"/>
         <v>561</v>
       </c>
-      <c r="B563" s="21">
+      <c r="B563" s="5">
         <v>44482.0</v>
       </c>
       <c r="C563" s="2"/>
@@ -18833,7 +19011,7 @@
         <f t="shared" si="1"/>
         <v>562</v>
       </c>
-      <c r="B564" s="21">
+      <c r="B564" s="5">
         <v>44483.0</v>
       </c>
       <c r="C564" s="2"/>
@@ -18853,7 +19031,7 @@
         <f t="shared" si="1"/>
         <v>563</v>
       </c>
-      <c r="B565" s="21">
+      <c r="B565" s="5">
         <v>44484.0</v>
       </c>
       <c r="C565" s="2"/>
@@ -18873,7 +19051,7 @@
         <f t="shared" si="1"/>
         <v>564</v>
       </c>
-      <c r="B566" s="21">
+      <c r="B566" s="5">
         <v>44485.0</v>
       </c>
       <c r="C566" s="2"/>
@@ -18893,7 +19071,7 @@
         <f t="shared" si="1"/>
         <v>565</v>
       </c>
-      <c r="B567" s="21">
+      <c r="B567" s="5">
         <v>44486.0</v>
       </c>
       <c r="C567" s="2"/>
@@ -18913,7 +19091,7 @@
         <f t="shared" si="1"/>
         <v>566</v>
       </c>
-      <c r="B568" s="21">
+      <c r="B568" s="5">
         <v>44487.0</v>
       </c>
       <c r="C568" s="2"/>
@@ -18933,7 +19111,7 @@
         <f t="shared" si="1"/>
         <v>567</v>
       </c>
-      <c r="B569" s="21">
+      <c r="B569" s="5">
         <v>44488.0</v>
       </c>
       <c r="C569" s="2"/>
@@ -18953,7 +19131,7 @@
         <f t="shared" si="1"/>
         <v>568</v>
       </c>
-      <c r="B570" s="21">
+      <c r="B570" s="5">
         <v>44489.0</v>
       </c>
       <c r="C570" s="2"/>
@@ -18973,7 +19151,7 @@
         <f t="shared" si="1"/>
         <v>569</v>
       </c>
-      <c r="B571" s="21">
+      <c r="B571" s="5">
         <v>44490.0</v>
       </c>
       <c r="C571" s="2"/>
@@ -18993,7 +19171,7 @@
         <f t="shared" si="1"/>
         <v>570</v>
       </c>
-      <c r="B572" s="21">
+      <c r="B572" s="5">
         <v>44491.0</v>
       </c>
       <c r="C572" s="2"/>
@@ -19013,7 +19191,7 @@
         <f t="shared" si="1"/>
         <v>571</v>
       </c>
-      <c r="B573" s="21">
+      <c r="B573" s="5">
         <v>44492.0</v>
       </c>
       <c r="C573" s="2"/>
@@ -19033,7 +19211,7 @@
         <f t="shared" si="1"/>
         <v>572</v>
       </c>
-      <c r="B574" s="21">
+      <c r="B574" s="5">
         <v>44493.0</v>
       </c>
       <c r="C574" s="2"/>
@@ -19053,7 +19231,7 @@
         <f t="shared" si="1"/>
         <v>573</v>
       </c>
-      <c r="B575" s="21">
+      <c r="B575" s="5">
         <v>44494.0</v>
       </c>
       <c r="C575" s="2"/>
@@ -19073,7 +19251,7 @@
         <f t="shared" si="1"/>
         <v>574</v>
       </c>
-      <c r="B576" s="21">
+      <c r="B576" s="5">
         <v>44495.0</v>
       </c>
       <c r="C576" s="2"/>
@@ -19093,7 +19271,7 @@
         <f t="shared" si="1"/>
         <v>575</v>
       </c>
-      <c r="B577" s="21">
+      <c r="B577" s="5">
         <v>44496.0</v>
       </c>
       <c r="C577" s="2"/>
@@ -19113,7 +19291,7 @@
         <f t="shared" si="1"/>
         <v>576</v>
       </c>
-      <c r="B578" s="21">
+      <c r="B578" s="5">
         <v>44497.0</v>
       </c>
       <c r="C578" s="2"/>
@@ -19133,7 +19311,7 @@
         <f t="shared" si="1"/>
         <v>577</v>
       </c>
-      <c r="B579" s="21">
+      <c r="B579" s="5">
         <v>44498.0</v>
       </c>
       <c r="C579" s="2"/>
@@ -19153,7 +19331,7 @@
         <f t="shared" si="1"/>
         <v>578</v>
       </c>
-      <c r="B580" s="21">
+      <c r="B580" s="5">
         <v>44499.0</v>
       </c>
       <c r="C580" s="2"/>
@@ -19173,7 +19351,7 @@
         <f t="shared" si="1"/>
         <v>579</v>
       </c>
-      <c r="B581" s="21">
+      <c r="B581" s="5">
         <v>44500.0</v>
       </c>
       <c r="C581" s="2"/>
@@ -19189,7 +19367,7 @@
       <c r="M581" s="2"/>
     </row>
     <row r="582" ht="15.75" customHeight="1">
-      <c r="A582" s="19"/>
+      <c r="A582" s="1"/>
     </row>
     <row r="583" ht="15.75" customHeight="1"/>
     <row r="584" ht="15.75" customHeight="1"/>
@@ -19611,7 +19789,7 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{B5C5D958-6324-40D8-B4E1-76BBA7389C94}" filter="1" showAutoFilter="1">
+    <customSheetView guid="{D43912C3-DA06-41C2-8E8C-8C4107953FBA}" filter="1" showAutoFilter="1">
       <autoFilter ref="$G$9"/>
       <extLst>
         <ext uri="GoogleSheetsCustomDataVersion1">

</xml_diff>